<commit_message>
added missing core measure section names
</commit_message>
<xml_diff>
--- a/xlsx/core_measures.xlsx
+++ b/xlsx/core_measures.xlsx
@@ -889,7 +889,11 @@
       <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Demographics</t>
+        </is>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
           <t>d1</t>
@@ -925,7 +929,11 @@
       <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Demographics</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>d1a</t>
@@ -957,7 +965,11 @@
       <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Demographics</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>o1</t>

</xml_diff>

<commit_message>
tabular format csvs with new variable names
</commit_message>
<xml_diff>
--- a/xlsx/core_measures.xlsx
+++ b/xlsx/core_measures.xlsx
@@ -621,7 +621,7 @@
     <col width="20" customWidth="1" min="9" max="9"/>
     <col width="21" customWidth="1" min="10" max="10"/>
     <col width="41" customWidth="1" min="11" max="11"/>
-    <col width="34" customWidth="1" min="12" max="12"/>
+    <col width="26" customWidth="1" min="12" max="12"/>
     <col width="6" customWidth="1" min="13" max="13"/>
     <col width="171" customWidth="1" min="14" max="14"/>
   </cols>
@@ -836,7 +836,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>state of site</t>
+          <t>state_of_site_enrollment</t>
         </is>
       </c>
       <c r="M4" t="inlineStr"/>
@@ -920,7 +920,11 @@
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>birth_date</t>
+        </is>
+      </c>
       <c r="M6" t="inlineStr">
         <is>
           <t>%Y%m%d</t>
@@ -960,7 +964,11 @@
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>age</t>
+        </is>
+      </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
     </row>
@@ -1000,7 +1008,11 @@
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>sex_at_birth</t>
+        </is>
+      </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
     </row>
@@ -1042,7 +1054,7 @@
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>gender_identity_long</t>
+          <t>gender_id</t>
         </is>
       </c>
       <c r="M9" t="inlineStr"/>
@@ -1091,7 +1103,7 @@
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
         <is>
-          <t>gender identity_short</t>
+          <t>gender_id_condensed</t>
         </is>
       </c>
       <c r="M10" t="inlineStr"/>
@@ -1245,7 +1257,7 @@
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
-          <t>race_american_indian</t>
+          <t>race_AIAN</t>
         </is>
       </c>
       <c r="M13" t="inlineStr"/>
@@ -1295,7 +1307,7 @@
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
-          <t>race_hawaiian</t>
+          <t>race_hawaiian_OPI</t>
         </is>
       </c>
       <c r="M14" t="inlineStr"/>
@@ -1437,7 +1449,7 @@
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
-          <t>race_specify_american_indian_tribe</t>
+          <t>race_AI_tribe</t>
         </is>
       </c>
       <c r="M17" t="inlineStr"/>
@@ -1479,7 +1491,7 @@
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
-          <t>race_specify_other</t>
+          <t>race_other_specified</t>
         </is>
       </c>
       <c r="M18" t="inlineStr"/>
@@ -1529,7 +1541,7 @@
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
-          <t>hispanic</t>
+          <t>hispanic_latino</t>
         </is>
       </c>
       <c r="M19" t="inlineStr"/>
@@ -1573,7 +1585,7 @@
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
-          <t>sexual_orientation</t>
+          <t>sex_orient_category</t>
         </is>
       </c>
       <c r="M20" t="inlineStr"/>
@@ -1613,7 +1625,7 @@
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
-          <t>sexual_orientation_other</t>
+          <t>sex_orient_other</t>
         </is>
       </c>
       <c r="M21" t="inlineStr"/>
@@ -1657,7 +1669,7 @@
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr">
         <is>
-          <t>pregnant</t>
+          <t>ever_pregnant</t>
         </is>
       </c>
       <c r="M22" t="inlineStr"/>
@@ -1749,7 +1761,7 @@
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr">
         <is>
-          <t>unmarried_partner</t>
+          <t>living_as_married</t>
         </is>
       </c>
       <c r="M24" t="inlineStr"/>
@@ -1793,7 +1805,7 @@
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>educ_category</t>
         </is>
       </c>
       <c r="M25" t="inlineStr"/>
@@ -1833,7 +1845,7 @@
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr">
         <is>
-          <t>education_grade</t>
+          <t>educ_highest_grade</t>
         </is>
       </c>
       <c r="M26" t="inlineStr"/>
@@ -1873,7 +1885,7 @@
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
-          <t>education_other</t>
+          <t>educ_other_specified</t>
         </is>
       </c>
       <c r="M27" t="inlineStr"/>
@@ -1921,7 +1933,7 @@
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr">
         <is>
-          <t>iv_incarceration</t>
+          <t>intv_while_incarc</t>
         </is>
       </c>
       <c r="M28" t="inlineStr"/>
@@ -1961,7 +1973,7 @@
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr">
         <is>
-          <t>incarceration_days</t>
+          <t>days_incarcerated_interval</t>
         </is>
       </c>
       <c r="M29" t="inlineStr"/>
@@ -2009,7 +2021,7 @@
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr">
         <is>
-          <t>oud_meds_rx</t>
+          <t>ever_rx_moud</t>
         </is>
       </c>
       <c r="M30" t="inlineStr"/>
@@ -2049,7 +2061,7 @@
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr">
         <is>
-          <t>buprenorphine_tab_mos</t>
+          <t>months_daily_bup</t>
         </is>
       </c>
       <c r="M31" t="inlineStr"/>
@@ -2089,7 +2101,7 @@
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>sublocade_mos</t>
+          <t>months_sublocade</t>
         </is>
       </c>
       <c r="M32" t="inlineStr"/>
@@ -2129,7 +2141,7 @@
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
         <is>
-          <t>brixadi_weekly_mos</t>
+          <t>months_weekly_brixadi</t>
         </is>
       </c>
       <c r="M33" t="inlineStr"/>
@@ -2169,7 +2181,7 @@
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr">
         <is>
-          <t>brixadi_monthly_mos</t>
+          <t>months_monthly_brixadi</t>
         </is>
       </c>
       <c r="M34" t="inlineStr"/>
@@ -2209,7 +2221,7 @@
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr">
         <is>
-          <t>probuphine_mos</t>
+          <t>months_probuphine_implant</t>
         </is>
       </c>
       <c r="M35" t="inlineStr"/>
@@ -2249,7 +2261,7 @@
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr">
         <is>
-          <t>naltrexone_mos</t>
+          <t>months_daily_ntx</t>
         </is>
       </c>
       <c r="M36" t="inlineStr"/>
@@ -2289,7 +2301,7 @@
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr">
         <is>
-          <t>vivitrol_mos</t>
+          <t>months_monthly_vivitrol</t>
         </is>
       </c>
       <c r="M37" t="inlineStr"/>
@@ -2329,7 +2341,7 @@
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
-          <t>methadone_mos</t>
+          <t>months_methadone</t>
         </is>
       </c>
       <c r="M38" t="inlineStr"/>
@@ -5721,7 +5733,7 @@
     <col width="38.5" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
     <col width="22" customWidth="1" min="10" max="10"/>
-    <col width="51" customWidth="1" min="11" max="11"/>
+    <col width="32" customWidth="1" min="11" max="11"/>
     <col width="19" customWidth="1" min="12" max="12"/>
     <col width="6" customWidth="1" min="13" max="13"/>
     <col width="259" customWidth="1" min="14" max="14"/>
@@ -5932,7 +5944,7 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t>shifted_visit_dt</t>
+          <t>shifted_visit_date</t>
         </is>
       </c>
       <c r="L4" t="inlineStr"/>
@@ -6077,7 +6089,7 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
-          <t>last_drug_get_use_recover</t>
+          <t>last_getting_using_drugs</t>
         </is>
       </c>
       <c r="L7" t="inlineStr"/>
@@ -6126,7 +6138,7 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
         <is>
-          <t>last_drug_use_social_dysfunction</t>
+          <t>last_social_problems</t>
         </is>
       </c>
       <c r="L8" t="inlineStr"/>
@@ -6175,7 +6187,7 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
-          <t>last_drug_use_work_life_dysfunction</t>
+          <t>last_work_life_disruption</t>
         </is>
       </c>
       <c r="L9" t="inlineStr"/>
@@ -6224,7 +6236,7 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
-          <t>last_drug_use_withdrawal</t>
+          <t>last_withdrawal</t>
         </is>
       </c>
       <c r="L10" t="inlineStr"/>
@@ -6273,7 +6285,7 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
-          <t>last_time_opioid_use</t>
+          <t>last_used_opioids</t>
         </is>
       </c>
       <c r="L11" t="inlineStr"/>
@@ -6322,7 +6334,7 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr">
         <is>
-          <t>last_time_opioid_overdose</t>
+          <t>last_opioid_overdose</t>
         </is>
       </c>
       <c r="L12" t="inlineStr"/>
@@ -6371,7 +6383,7 @@
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
-          <t>last_time_opioid_med_treatment</t>
+          <t>last_went_moud</t>
         </is>
       </c>
       <c r="L13" t="inlineStr"/>
@@ -6416,7 +6428,7 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
-          <t>opioid_overdose_ct</t>
+          <t>times_opioid_overdose</t>
         </is>
       </c>
       <c r="L14" t="inlineStr"/>
@@ -6461,7 +6473,7 @@
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr">
         <is>
-          <t>opioid_overdose_naloxone_ct</t>
+          <t>times_naloxone</t>
         </is>
       </c>
       <c r="L15" t="inlineStr"/>
@@ -6506,7 +6518,7 @@
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
-          <t>who_administered_naloxone</t>
+          <t>who_gave_naloxone</t>
         </is>
       </c>
       <c r="L16" t="inlineStr"/>
@@ -6551,7 +6563,7 @@
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr">
         <is>
-          <t>drugs_4hrs_prior_to_overdose</t>
+          <t>drugs_before_overdose</t>
         </is>
       </c>
       <c r="L17" t="inlineStr"/>
@@ -6596,7 +6608,7 @@
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr">
         <is>
-          <t>emergency_service_after_overdose</t>
+          <t>times_ems_after_overdose</t>
         </is>
       </c>
       <c r="L18" t="inlineStr"/>
@@ -6637,7 +6649,7 @@
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr">
         <is>
-          <t>emergency_dept_after_overdose_ct</t>
+          <t>times_er_after_overdose</t>
         </is>
       </c>
       <c r="L19" t="inlineStr"/>
@@ -6678,7 +6690,7 @@
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr">
         <is>
-          <t>hospital_admission_after_overdose_ct</t>
+          <t>times_hospital_after_overdose</t>
         </is>
       </c>
       <c r="L20" t="inlineStr"/>
@@ -6719,7 +6731,7 @@
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr">
         <is>
-          <t>substance_use_treatment_referral_ct</t>
+          <t>tx_refer_after_overdose</t>
         </is>
       </c>
       <c r="L21" t="inlineStr"/>
@@ -6760,7 +6772,7 @@
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr">
         <is>
-          <t>drug_use_ct</t>
+          <t>days_drug_use</t>
         </is>
       </c>
       <c r="L22" t="inlineStr"/>
@@ -6801,7 +6813,7 @@
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr">
         <is>
-          <t>alcohol_use_ct</t>
+          <t>days_alcohol_use</t>
         </is>
       </c>
       <c r="L23" t="inlineStr"/>
@@ -6842,7 +6854,7 @@
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr">
         <is>
-          <t>alcohol_binge_ct</t>
+          <t>days_alcohol_binge</t>
         </is>
       </c>
       <c r="L24" t="inlineStr"/>
@@ -6883,7 +6895,7 @@
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr">
         <is>
-          <t>marijuana_medical_use_ct</t>
+          <t>days_medical_marijuana</t>
         </is>
       </c>
       <c r="L25" t="inlineStr"/>
@@ -6924,7 +6936,7 @@
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr">
         <is>
-          <t>marijuana_not_own_use_ct</t>
+          <t>days_other_marijuana</t>
         </is>
       </c>
       <c r="L26" t="inlineStr"/>
@@ -6965,7 +6977,7 @@
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr">
         <is>
-          <t>opioid_heroin_use_ct</t>
+          <t>days_heroin</t>
         </is>
       </c>
       <c r="L27" t="inlineStr"/>
@@ -7006,7 +7018,7 @@
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr">
         <is>
-          <t>opioid_fentanyl_use_ct</t>
+          <t>days_fentanyl</t>
         </is>
       </c>
       <c r="L28" t="inlineStr"/>
@@ -7047,7 +7059,7 @@
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr">
         <is>
-          <t>opioid_street_methadone_use_ct</t>
+          <t>days_non_rx_methadone</t>
         </is>
       </c>
       <c r="L29" t="inlineStr"/>
@@ -7088,7 +7100,7 @@
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr">
         <is>
-          <t>opioid_suboxone_use_ct</t>
+          <t>days_non_rx_suboxone</t>
         </is>
       </c>
       <c r="L30" t="inlineStr"/>
@@ -7129,7 +7141,7 @@
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr">
         <is>
-          <t>opioid_other_use_ct</t>
+          <t>days_other_opioids</t>
         </is>
       </c>
       <c r="L31" t="inlineStr"/>
@@ -7170,7 +7182,7 @@
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr">
         <is>
-          <t>cocaine_use_ct</t>
+          <t>days_cocaine</t>
         </is>
       </c>
       <c r="L32" t="inlineStr"/>
@@ -7211,7 +7223,7 @@
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr">
         <is>
-          <t>speed_use_ct</t>
+          <t>days_amphetamines</t>
         </is>
       </c>
       <c r="L33" t="inlineStr"/>
@@ -7252,7 +7264,7 @@
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr">
         <is>
-          <t>benzos_anti_anxiety_use_ct</t>
+          <t>days_benzo</t>
         </is>
       </c>
       <c r="L34" t="inlineStr"/>
@@ -7293,7 +7305,7 @@
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr">
         <is>
-          <t>drug_use_other_ct</t>
+          <t>days_other_drugs</t>
         </is>
       </c>
       <c r="L35" t="inlineStr"/>
@@ -7334,7 +7346,7 @@
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr">
         <is>
-          <t>drug_use_other_desc</t>
+          <t>other_drug_describe</t>
         </is>
       </c>
       <c r="L36" t="inlineStr"/>
@@ -7375,7 +7387,7 @@
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr">
         <is>
-          <t>place_of_no_drug_use_ct</t>
+          <t>days_confined_no_use</t>
         </is>
       </c>
       <c r="L37" t="inlineStr"/>
@@ -7416,7 +7428,7 @@
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr">
         <is>
-          <t>activities_against_law_besides_drugs_ct</t>
+          <t>days_illegal_activity</t>
         </is>
       </c>
       <c r="L38" t="inlineStr"/>
@@ -7461,7 +7473,7 @@
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr">
         <is>
-          <t>drug_possession_ct</t>
+          <t>times_drug_possession</t>
         </is>
       </c>
       <c r="L39" t="inlineStr"/>
@@ -7506,7 +7518,7 @@
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr">
         <is>
-          <t>drunkenness_or_other_liquor_law_violations_ct</t>
+          <t>times_public_drunk</t>
         </is>
       </c>
       <c r="L40" t="inlineStr"/>
@@ -7551,7 +7563,7 @@
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr">
         <is>
-          <t>driving_under_the_influence_or_while_intoxicated_ct</t>
+          <t>times_dui</t>
         </is>
       </c>
       <c r="L41" t="inlineStr"/>
@@ -7596,7 +7608,7 @@
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr">
         <is>
-          <t>possession_dealing_distribution_or_sale_of_drugs_ct</t>
+          <t>times_drug_dealing</t>
         </is>
       </c>
       <c r="L42" t="inlineStr"/>
@@ -7641,7 +7653,7 @@
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr">
         <is>
-          <t>vandalism_or_property_destruction_ct</t>
+          <t>times_vandalism</t>
         </is>
       </c>
       <c r="L43" t="inlineStr"/>
@@ -7686,7 +7698,7 @@
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr">
         <is>
-          <t>receiving_possessing_or_selling_stolen_goods_ct</t>
+          <t>times_stolen_goods</t>
         </is>
       </c>
       <c r="L44" t="inlineStr"/>
@@ -7731,7 +7743,7 @@
       <c r="J45" t="inlineStr"/>
       <c r="K45" t="inlineStr">
         <is>
-          <t>forgery_fraud_or_embezzlement_ct</t>
+          <t>times_forgery</t>
         </is>
       </c>
       <c r="L45" t="inlineStr"/>
@@ -7776,7 +7788,7 @@
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr">
         <is>
-          <t>shoplifting_ct</t>
+          <t>times_shoplift</t>
         </is>
       </c>
       <c r="L46" t="inlineStr"/>
@@ -7821,7 +7833,7 @@
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr">
         <is>
-          <t>larceny_or_theft_ct</t>
+          <t>times_theft</t>
         </is>
       </c>
       <c r="L47" t="inlineStr"/>
@@ -7866,7 +7878,7 @@
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr">
         <is>
-          <t>burglary_or_breaking_and_entering_ct</t>
+          <t>times_burglary</t>
         </is>
       </c>
       <c r="L48" t="inlineStr"/>
@@ -7911,7 +7923,7 @@
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="inlineStr">
         <is>
-          <t>motor_vehicle_theft_ct</t>
+          <t>times_auto_theft</t>
         </is>
       </c>
       <c r="L49" t="inlineStr"/>
@@ -7956,7 +7968,7 @@
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="inlineStr">
         <is>
-          <t>carjacking_ct</t>
+          <t>times_carjacking</t>
         </is>
       </c>
       <c r="L50" t="inlineStr"/>
@@ -8001,7 +8013,7 @@
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="inlineStr">
         <is>
-          <t>simple_assault_or_battery_ct</t>
+          <t>times_assault</t>
         </is>
       </c>
       <c r="L51" t="inlineStr"/>
@@ -8046,7 +8058,7 @@
       <c r="J52" t="inlineStr"/>
       <c r="K52" t="inlineStr">
         <is>
-          <t>robbery_ct</t>
+          <t>times_robbery</t>
         </is>
       </c>
       <c r="L52" t="inlineStr"/>
@@ -8091,7 +8103,7 @@
       <c r="J53" t="inlineStr"/>
       <c r="K53" t="inlineStr">
         <is>
-          <t>aggravated_assault_or_battery_ct</t>
+          <t>times_aggravated_assault</t>
         </is>
       </c>
       <c r="L53" t="inlineStr"/>
@@ -8136,7 +8148,7 @@
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="inlineStr">
         <is>
-          <t>forcible_rape_ct</t>
+          <t>times_rape</t>
         </is>
       </c>
       <c r="L54" t="inlineStr"/>
@@ -8181,7 +8193,7 @@
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr">
         <is>
-          <t>murder_homicide_or_no-negligent_manslaughter_ct</t>
+          <t>times_homicide</t>
         </is>
       </c>
       <c r="L55" t="inlineStr"/>
@@ -8226,7 +8238,7 @@
       <c r="J56" t="inlineStr"/>
       <c r="K56" t="inlineStr">
         <is>
-          <t>arson_ct</t>
+          <t>times_arson</t>
         </is>
       </c>
       <c r="L56" t="inlineStr"/>
@@ -8271,7 +8283,7 @@
       <c r="J57" t="inlineStr"/>
       <c r="K57" t="inlineStr">
         <is>
-          <t>prostitution_pimping_or_commercialized_sex_ct</t>
+          <t>times_prostitution</t>
         </is>
       </c>
       <c r="L57" t="inlineStr"/>
@@ -8316,7 +8328,7 @@
       <c r="J58" t="inlineStr"/>
       <c r="K58" t="inlineStr">
         <is>
-          <t>other_unlawful_activities_ct</t>
+          <t>times_other_unlawful</t>
         </is>
       </c>
       <c r="L58" t="inlineStr"/>
@@ -8361,7 +8373,7 @@
       <c r="J59" t="inlineStr"/>
       <c r="K59" t="inlineStr">
         <is>
-          <t>overall_charged_arrests_ct</t>
+          <t>number_charged_arrests</t>
         </is>
       </c>
       <c r="L59" t="inlineStr"/>
@@ -8402,7 +8414,7 @@
       <c r="J60" t="inlineStr"/>
       <c r="K60" t="inlineStr">
         <is>
-          <t>drug_possession_arrests_ct</t>
+          <t>number_arrest_possession</t>
         </is>
       </c>
       <c r="L60" t="inlineStr"/>
@@ -8443,7 +8455,7 @@
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="inlineStr">
         <is>
-          <t>law_violations_arrests_ct</t>
+          <t>number_arrest_drunk</t>
         </is>
       </c>
       <c r="L61" t="inlineStr"/>
@@ -8484,7 +8496,7 @@
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="inlineStr">
         <is>
-          <t>driving_under_the_influence/intoxicated_arrests_ct</t>
+          <t>number_arrest_dui</t>
         </is>
       </c>
       <c r="L62" t="inlineStr"/>
@@ -8525,7 +8537,7 @@
       <c r="J63" t="inlineStr"/>
       <c r="K63" t="inlineStr">
         <is>
-          <t>drug_activity_arrests_ct</t>
+          <t>number_arrest_drug_dealing</t>
         </is>
       </c>
       <c r="L63" t="inlineStr"/>
@@ -8566,7 +8578,7 @@
       <c r="J64" t="inlineStr"/>
       <c r="K64" t="inlineStr">
         <is>
-          <t>vandalism_or_property_destruction_arrests_ct</t>
+          <t>number_arrest_vandalism</t>
         </is>
       </c>
       <c r="L64" t="inlineStr"/>
@@ -8607,7 +8619,7 @@
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="inlineStr">
         <is>
-          <t>stolen_goods_arrests_ct</t>
+          <t>number_arrest_stolen_goods</t>
         </is>
       </c>
       <c r="L65" t="inlineStr"/>
@@ -8648,7 +8660,7 @@
       <c r="J66" t="inlineStr"/>
       <c r="K66" t="inlineStr">
         <is>
-          <t>forgery_fraud_or_embezzlement_arrests_ct</t>
+          <t>number_arrest_forgery</t>
         </is>
       </c>
       <c r="L66" t="inlineStr"/>
@@ -8689,7 +8701,7 @@
       <c r="J67" t="inlineStr"/>
       <c r="K67" t="inlineStr">
         <is>
-          <t>shoplifting_arrests_ct</t>
+          <t>number_arrest_shoplifting</t>
         </is>
       </c>
       <c r="L67" t="inlineStr"/>
@@ -8730,7 +8742,7 @@
       <c r="J68" t="inlineStr"/>
       <c r="K68" t="inlineStr">
         <is>
-          <t>theft_larceny_arrests_ct</t>
+          <t>number_arrest_theft</t>
         </is>
       </c>
       <c r="L68" t="inlineStr"/>
@@ -8771,7 +8783,7 @@
       <c r="J69" t="inlineStr"/>
       <c r="K69" t="inlineStr">
         <is>
-          <t>burglary_or_breaking_and_entering_arrests_ct</t>
+          <t>number_arrest_burglary</t>
         </is>
       </c>
       <c r="L69" t="inlineStr"/>
@@ -8812,7 +8824,7 @@
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="inlineStr">
         <is>
-          <t>vehicle_theft_arrests_ct</t>
+          <t>number_arrest_auto_theft</t>
         </is>
       </c>
       <c r="L70" t="inlineStr"/>
@@ -8853,7 +8865,7 @@
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="inlineStr">
         <is>
-          <t>car_jacking_arrests_ct</t>
+          <t>number_arrest_carjacking</t>
         </is>
       </c>
       <c r="L71" t="inlineStr"/>
@@ -8894,7 +8906,7 @@
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="inlineStr">
         <is>
-          <t>simple_assault_or_battery_arrests_ct</t>
+          <t>number_arrest_assault</t>
         </is>
       </c>
       <c r="L72" t="inlineStr"/>
@@ -8935,7 +8947,7 @@
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr">
         <is>
-          <t>robbery_arrests_ct</t>
+          <t>number_arrest_robbery</t>
         </is>
       </c>
       <c r="L73" t="inlineStr"/>
@@ -8976,7 +8988,7 @@
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr">
         <is>
-          <t>aggravated_assault_or_battery_arrests_ct</t>
+          <t>number_arrest_aggravated</t>
         </is>
       </c>
       <c r="L74" t="inlineStr"/>
@@ -9017,7 +9029,7 @@
       <c r="J75" t="inlineStr"/>
       <c r="K75" t="inlineStr">
         <is>
-          <t>forcible_rape_arrests_ct</t>
+          <t>number_arrest_rape</t>
         </is>
       </c>
       <c r="L75" t="inlineStr"/>
@@ -9058,7 +9070,7 @@
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr">
         <is>
-          <t>negligent_manslaughter_arrests_ct</t>
+          <t>number_arrest_homicide</t>
         </is>
       </c>
       <c r="L76" t="inlineStr"/>
@@ -9099,7 +9111,7 @@
       <c r="J77" t="inlineStr"/>
       <c r="K77" t="inlineStr">
         <is>
-          <t>arson_arrests_ct</t>
+          <t>number_arrest_arson</t>
         </is>
       </c>
       <c r="L77" t="inlineStr"/>
@@ -9140,7 +9152,7 @@
       <c r="J78" t="inlineStr"/>
       <c r="K78" t="inlineStr">
         <is>
-          <t>commercialized_sex_arrests_ct</t>
+          <t>number_arrest_prostitution</t>
         </is>
       </c>
       <c r="L78" t="inlineStr"/>
@@ -9181,7 +9193,7 @@
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="inlineStr">
         <is>
-          <t>other_charges_arrests_ct</t>
+          <t>number_arrest_other</t>
         </is>
       </c>
       <c r="L79" t="inlineStr"/>
@@ -9222,7 +9234,7 @@
       <c r="J80" t="inlineStr"/>
       <c r="K80" t="inlineStr">
         <is>
-          <t>num_days_electronic_monitoring</t>
+          <t>days_electronic_monitoring</t>
         </is>
       </c>
       <c r="L80" t="inlineStr"/>
@@ -9263,7 +9275,7 @@
       <c r="J81" t="inlineStr"/>
       <c r="K81" t="inlineStr">
         <is>
-          <t>num_days_house_arrest</t>
+          <t>days_house_arrest</t>
         </is>
       </c>
       <c r="L81" t="inlineStr"/>
@@ -9304,7 +9316,7 @@
       <c r="J82" t="inlineStr"/>
       <c r="K82" t="inlineStr">
         <is>
-          <t>num_days_jail_time</t>
+          <t>days_jail</t>
         </is>
       </c>
       <c r="L82" t="inlineStr"/>
@@ -9345,7 +9357,7 @@
       <c r="J83" t="inlineStr"/>
       <c r="K83" t="inlineStr">
         <is>
-          <t>num_days_prison_time</t>
+          <t>days_prison</t>
         </is>
       </c>
       <c r="L83" t="inlineStr"/>
@@ -9394,7 +9406,7 @@
       <c r="J84" t="inlineStr"/>
       <c r="K84" t="inlineStr">
         <is>
-          <t>current_jail_or_prison_ind</t>
+          <t>currently_incarcerated</t>
         </is>
       </c>
       <c r="L84" t="inlineStr"/>
@@ -9439,7 +9451,7 @@
       <c r="J85" t="inlineStr"/>
       <c r="K85" t="inlineStr">
         <is>
-          <t>length_of_jail_or_prison_time</t>
+          <t>length_current_incarceration</t>
         </is>
       </c>
       <c r="L85" t="inlineStr"/>
@@ -9480,7 +9492,7 @@
       <c r="J86" t="inlineStr"/>
       <c r="K86" t="inlineStr">
         <is>
-          <t>num_days_parole</t>
+          <t>days_parole</t>
         </is>
       </c>
       <c r="L86" t="inlineStr"/>
@@ -9521,7 +9533,7 @@
       <c r="J87" t="inlineStr"/>
       <c r="K87" t="inlineStr">
         <is>
-          <t>num_days_probation</t>
+          <t>days_probation</t>
         </is>
       </c>
       <c r="L87" t="inlineStr"/>
@@ -9562,7 +9574,7 @@
       <c r="J88" t="inlineStr"/>
       <c r="K88" t="inlineStr">
         <is>
-          <t>num_days_other_kind_of_community_supervision</t>
+          <t>days_other_supervision</t>
         </is>
       </c>
       <c r="L88" t="inlineStr"/>
@@ -9603,7 +9615,7 @@
       <c r="J89" t="inlineStr"/>
       <c r="K89" t="inlineStr">
         <is>
-          <t>num_days_meeting_with_probation_or_parole_officer</t>
+          <t>days_met_probation_officer</t>
         </is>
       </c>
       <c r="L89" t="inlineStr"/>
@@ -9644,7 +9656,7 @@
       <c r="J90" t="inlineStr"/>
       <c r="K90" t="inlineStr">
         <is>
-          <t>num_days_trouble_with_probation_or_parole_officer</t>
+          <t>days_trouble_probation_officer</t>
         </is>
       </c>
       <c r="L90" t="inlineStr"/>
@@ -9685,7 +9697,7 @@
       <c r="J91" t="inlineStr"/>
       <c r="K91" t="inlineStr">
         <is>
-          <t>num_days_life_time_arrests</t>
+          <t>number_lifetime_arrests</t>
         </is>
       </c>
       <c r="L91" t="inlineStr"/>
@@ -9726,7 +9738,7 @@
       <c r="J92" t="inlineStr"/>
       <c r="K92" t="inlineStr">
         <is>
-          <t>age_at_first_time_arrest</t>
+          <t>age_first_arrest</t>
         </is>
       </c>
       <c r="L92" t="inlineStr"/>
@@ -9767,7 +9779,7 @@
       <c r="J93" t="inlineStr"/>
       <c r="K93" t="inlineStr">
         <is>
-          <t>lifetime_years_in_detention_jail_or_prison_time_ct</t>
+          <t>years_lifetime_incarceration</t>
         </is>
       </c>
       <c r="L93" t="inlineStr"/>
@@ -9812,7 +9824,7 @@
       <c r="J94" t="inlineStr"/>
       <c r="K94" t="inlineStr">
         <is>
-          <t>lifetime_months_in_detention_jail_or_prison_time_ct</t>
+          <t>months_lifetime_incarceration</t>
         </is>
       </c>
       <c r="L94" t="inlineStr"/>
@@ -9857,7 +9869,7 @@
       <c r="J95" t="inlineStr"/>
       <c r="K95" t="inlineStr">
         <is>
-          <t>lifetime_guity_and_sentenced_ct</t>
+          <t>times_guilty_sentenced</t>
         </is>
       </c>
       <c r="L95" t="inlineStr"/>
@@ -9898,7 +9910,7 @@
       <c r="J96" t="inlineStr"/>
       <c r="K96" t="inlineStr">
         <is>
-          <t>first_time_adjudication_conviction_ct</t>
+          <t>age_first_convicted</t>
         </is>
       </c>
       <c r="L96" t="inlineStr"/>
@@ -9937,7 +9949,11 @@
       </c>
       <c r="I97" t="inlineStr"/>
       <c r="J97" t="inlineStr"/>
-      <c r="K97" t="inlineStr"/>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>times_er_visits</t>
+        </is>
+      </c>
       <c r="L97" t="inlineStr"/>
       <c r="M97" t="inlineStr"/>
       <c r="N97" t="inlineStr"/>
@@ -9974,7 +9990,11 @@
       </c>
       <c r="I98" t="inlineStr"/>
       <c r="J98" t="inlineStr"/>
-      <c r="K98" t="inlineStr"/>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>nights_hospital_detox</t>
+        </is>
+      </c>
       <c r="L98" t="inlineStr"/>
       <c r="M98" t="inlineStr"/>
       <c r="N98" t="inlineStr"/>
@@ -10011,7 +10031,11 @@
       </c>
       <c r="I99" t="inlineStr"/>
       <c r="J99" t="inlineStr"/>
-      <c r="K99" t="inlineStr"/>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>nights_hospitalized</t>
+        </is>
+      </c>
       <c r="L99" t="inlineStr"/>
       <c r="M99" t="inlineStr"/>
       <c r="N99" t="inlineStr"/>
@@ -10048,7 +10072,11 @@
       </c>
       <c r="I100" t="inlineStr"/>
       <c r="J100" t="inlineStr"/>
-      <c r="K100" t="inlineStr"/>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>nights_residential_detox</t>
+        </is>
+      </c>
       <c r="L100" t="inlineStr"/>
       <c r="M100" t="inlineStr"/>
       <c r="N100" t="inlineStr"/>
@@ -10085,7 +10113,11 @@
       </c>
       <c r="I101" t="inlineStr"/>
       <c r="J101" t="inlineStr"/>
-      <c r="K101" t="inlineStr"/>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>nights_residential_sud_tx</t>
+        </is>
+      </c>
       <c r="L101" t="inlineStr"/>
       <c r="M101" t="inlineStr"/>
       <c r="N101" t="inlineStr"/>
@@ -10122,7 +10154,11 @@
       </c>
       <c r="I102" t="inlineStr"/>
       <c r="J102" t="inlineStr"/>
-      <c r="K102" t="inlineStr"/>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>nights_residential_mh</t>
+        </is>
+      </c>
       <c r="L102" t="inlineStr"/>
       <c r="M102" t="inlineStr"/>
       <c r="N102" t="inlineStr"/>
@@ -10159,7 +10195,11 @@
       </c>
       <c r="I103" t="inlineStr"/>
       <c r="J103" t="inlineStr"/>
-      <c r="K103" t="inlineStr"/>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>nights_physical_rehab</t>
+        </is>
+      </c>
       <c r="L103" t="inlineStr"/>
       <c r="M103" t="inlineStr"/>
       <c r="N103" t="inlineStr"/>
@@ -10196,7 +10236,11 @@
       </c>
       <c r="I104" t="inlineStr"/>
       <c r="J104" t="inlineStr"/>
-      <c r="K104" t="inlineStr"/>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>visits_primary_care</t>
+        </is>
+      </c>
       <c r="L104" t="inlineStr"/>
       <c r="M104" t="inlineStr"/>
       <c r="N104" t="inlineStr"/>
@@ -10241,7 +10285,11 @@
       </c>
       <c r="I105" t="inlineStr"/>
       <c r="J105" t="inlineStr"/>
-      <c r="K105" t="inlineStr"/>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>pc_reason_alc_drugs</t>
+        </is>
+      </c>
       <c r="L105" t="inlineStr"/>
       <c r="M105" t="inlineStr"/>
       <c r="N105" t="inlineStr"/>
@@ -10286,7 +10334,11 @@
       </c>
       <c r="I106" t="inlineStr"/>
       <c r="J106" t="inlineStr"/>
-      <c r="K106" t="inlineStr"/>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>pc_reason_mh</t>
+        </is>
+      </c>
       <c r="L106" t="inlineStr"/>
       <c r="M106" t="inlineStr"/>
       <c r="N106" t="inlineStr"/>
@@ -10331,7 +10383,11 @@
       </c>
       <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr"/>
-      <c r="K107" t="inlineStr"/>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>pc_reason_physical</t>
+        </is>
+      </c>
       <c r="L107" t="inlineStr"/>
       <c r="M107" t="inlineStr"/>
       <c r="N107" t="inlineStr"/>
@@ -10376,7 +10432,11 @@
       </c>
       <c r="I108" t="inlineStr"/>
       <c r="J108" t="inlineStr"/>
-      <c r="K108" t="inlineStr"/>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>pc_reason_other</t>
+        </is>
+      </c>
       <c r="L108" t="inlineStr"/>
       <c r="M108" t="inlineStr"/>
       <c r="N108" t="inlineStr"/>
@@ -10413,7 +10473,11 @@
       </c>
       <c r="I109" t="inlineStr"/>
       <c r="J109" t="inlineStr"/>
-      <c r="K109" t="inlineStr"/>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>pc_reason_other_specify</t>
+        </is>
+      </c>
       <c r="L109" t="inlineStr"/>
       <c r="M109" t="inlineStr"/>
       <c r="N109" t="inlineStr"/>
@@ -10450,7 +10514,11 @@
       </c>
       <c r="I110" t="inlineStr"/>
       <c r="J110" t="inlineStr"/>
-      <c r="K110" t="inlineStr"/>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>op_tx_days</t>
+        </is>
+      </c>
       <c r="L110" t="inlineStr"/>
       <c r="M110" t="inlineStr"/>
       <c r="N110" t="inlineStr"/>
@@ -10487,7 +10555,11 @@
       </c>
       <c r="I111" t="inlineStr"/>
       <c r="J111" t="inlineStr"/>
-      <c r="K111" t="inlineStr"/>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>op_tx_days_visited</t>
+        </is>
+      </c>
       <c r="L111" t="inlineStr"/>
       <c r="M111" t="inlineStr"/>
       <c r="N111" t="inlineStr"/>
@@ -10524,7 +10596,11 @@
       </c>
       <c r="I112" t="inlineStr"/>
       <c r="J112" t="inlineStr"/>
-      <c r="K112" t="inlineStr"/>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>op_tx_days_online</t>
+        </is>
+      </c>
       <c r="L112" t="inlineStr"/>
       <c r="M112" t="inlineStr"/>
       <c r="N112" t="inlineStr"/>
@@ -10561,7 +10637,11 @@
       </c>
       <c r="I113" t="inlineStr"/>
       <c r="J113" t="inlineStr"/>
-      <c r="K113" t="inlineStr"/>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>op_tx_days_doctor</t>
+        </is>
+      </c>
       <c r="L113" t="inlineStr"/>
       <c r="M113" t="inlineStr"/>
       <c r="N113" t="inlineStr"/>
@@ -10598,7 +10678,11 @@
       </c>
       <c r="I114" t="inlineStr"/>
       <c r="J114" t="inlineStr"/>
-      <c r="K114" t="inlineStr"/>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>op_tx_days_therapy</t>
+        </is>
+      </c>
       <c r="L114" t="inlineStr"/>
       <c r="M114" t="inlineStr"/>
       <c r="N114" t="inlineStr"/>
@@ -10635,7 +10719,11 @@
       </c>
       <c r="I115" t="inlineStr"/>
       <c r="J115" t="inlineStr"/>
-      <c r="K115" t="inlineStr"/>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>op_tx_days_moud_only</t>
+        </is>
+      </c>
       <c r="L115" t="inlineStr"/>
       <c r="M115" t="inlineStr"/>
       <c r="N115" t="inlineStr"/>
@@ -10672,7 +10760,11 @@
       </c>
       <c r="I116" t="inlineStr"/>
       <c r="J116" t="inlineStr"/>
-      <c r="K116" t="inlineStr"/>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>psych_visits</t>
+        </is>
+      </c>
       <c r="L116" t="inlineStr"/>
       <c r="M116" t="inlineStr"/>
       <c r="N116" t="inlineStr"/>
@@ -10709,7 +10801,11 @@
       </c>
       <c r="I117" t="inlineStr"/>
       <c r="J117" t="inlineStr"/>
-      <c r="K117" t="inlineStr"/>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>psych_visits_in_person</t>
+        </is>
+      </c>
       <c r="L117" t="inlineStr"/>
       <c r="M117" t="inlineStr"/>
       <c r="N117" t="inlineStr"/>
@@ -10746,7 +10842,11 @@
       </c>
       <c r="I118" t="inlineStr"/>
       <c r="J118" t="inlineStr"/>
-      <c r="K118" t="inlineStr"/>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>psych_visits_online</t>
+        </is>
+      </c>
       <c r="L118" t="inlineStr"/>
       <c r="M118" t="inlineStr"/>
       <c r="N118" t="inlineStr"/>
@@ -10783,7 +10883,11 @@
       </c>
       <c r="I119" t="inlineStr"/>
       <c r="J119" t="inlineStr"/>
-      <c r="K119" t="inlineStr"/>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>counselor_visits</t>
+        </is>
+      </c>
       <c r="L119" t="inlineStr"/>
       <c r="M119" t="inlineStr"/>
       <c r="N119" t="inlineStr"/>
@@ -10820,7 +10924,11 @@
       </c>
       <c r="I120" t="inlineStr"/>
       <c r="J120" t="inlineStr"/>
-      <c r="K120" t="inlineStr"/>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>counselor_visits_in_person</t>
+        </is>
+      </c>
       <c r="L120" t="inlineStr"/>
       <c r="M120" t="inlineStr"/>
       <c r="N120" t="inlineStr"/>
@@ -10857,7 +10965,11 @@
       </c>
       <c r="I121" t="inlineStr"/>
       <c r="J121" t="inlineStr"/>
-      <c r="K121" t="inlineStr"/>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>counselor_visits_online</t>
+        </is>
+      </c>
       <c r="L121" t="inlineStr"/>
       <c r="M121" t="inlineStr"/>
       <c r="N121" t="inlineStr"/>
@@ -10894,7 +11006,11 @@
       </c>
       <c r="I122" t="inlineStr"/>
       <c r="J122" t="inlineStr"/>
-      <c r="K122" t="inlineStr"/>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>healthcare_expense</t>
+        </is>
+      </c>
       <c r="L122" t="inlineStr"/>
       <c r="M122" t="inlineStr"/>
       <c r="N122" t="inlineStr"/>
@@ -10939,7 +11055,11 @@
       </c>
       <c r="I123" t="inlineStr"/>
       <c r="J123" t="inlineStr"/>
-      <c r="K123" t="inlineStr"/>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>received_sud_tx</t>
+        </is>
+      </c>
       <c r="L123" t="inlineStr"/>
       <c r="M123" t="inlineStr"/>
       <c r="N123" t="inlineStr"/>
@@ -10980,7 +11100,11 @@
       </c>
       <c r="I124" t="inlineStr"/>
       <c r="J124" t="inlineStr"/>
-      <c r="K124" t="inlineStr"/>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>sud_tx_organized</t>
+        </is>
+      </c>
       <c r="L124" t="inlineStr"/>
       <c r="M124" t="inlineStr"/>
       <c r="N124" t="inlineStr"/>
@@ -11021,7 +11145,11 @@
       </c>
       <c r="I125" t="inlineStr"/>
       <c r="J125" t="inlineStr"/>
-      <c r="K125" t="inlineStr"/>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>sud_tx_satisfied</t>
+        </is>
+      </c>
       <c r="L125" t="inlineStr"/>
       <c r="M125" t="inlineStr"/>
       <c r="N125" t="inlineStr"/>
@@ -11062,7 +11190,11 @@
       </c>
       <c r="I126" t="inlineStr"/>
       <c r="J126" t="inlineStr"/>
-      <c r="K126" t="inlineStr"/>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>sud_tx_efficient</t>
+        </is>
+      </c>
       <c r="L126" t="inlineStr"/>
       <c r="M126" t="inlineStr"/>
       <c r="N126" t="inlineStr"/>
@@ -11103,7 +11235,11 @@
       </c>
       <c r="I127" t="inlineStr"/>
       <c r="J127" t="inlineStr"/>
-      <c r="K127" t="inlineStr"/>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>sud_tx_personal</t>
+        </is>
+      </c>
       <c r="L127" t="inlineStr"/>
       <c r="M127" t="inlineStr"/>
       <c r="N127" t="inlineStr"/>
@@ -11144,7 +11280,11 @@
       </c>
       <c r="I128" t="inlineStr"/>
       <c r="J128" t="inlineStr"/>
-      <c r="K128" t="inlineStr"/>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>sud_tx_moud</t>
+        </is>
+      </c>
       <c r="L128" t="inlineStr"/>
       <c r="M128" t="inlineStr"/>
       <c r="N128" t="inlineStr"/>
@@ -11189,7 +11329,11 @@
       </c>
       <c r="I129" t="inlineStr"/>
       <c r="J129" t="inlineStr"/>
-      <c r="K129" t="inlineStr"/>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>oud_tx_not_appropriate</t>
+        </is>
+      </c>
       <c r="L129" t="inlineStr"/>
       <c r="M129" t="inlineStr"/>
       <c r="N129" t="inlineStr"/>
@@ -11234,7 +11378,11 @@
       </c>
       <c r="I130" t="inlineStr"/>
       <c r="J130" t="inlineStr"/>
-      <c r="K130" t="inlineStr"/>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>prefer_oud_meds</t>
+        </is>
+      </c>
       <c r="L130" t="inlineStr"/>
       <c r="M130" t="inlineStr"/>
       <c r="N130" t="inlineStr"/>
@@ -11279,7 +11427,11 @@
       </c>
       <c r="I131" t="inlineStr"/>
       <c r="J131" t="inlineStr"/>
-      <c r="K131" t="inlineStr"/>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>prefer_oud_detox</t>
+        </is>
+      </c>
       <c r="L131" t="inlineStr"/>
       <c r="M131" t="inlineStr"/>
       <c r="N131" t="inlineStr"/>
@@ -11324,7 +11476,11 @@
       </c>
       <c r="I132" t="inlineStr"/>
       <c r="J132" t="inlineStr"/>
-      <c r="K132" t="inlineStr"/>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>prefer_oud_op</t>
+        </is>
+      </c>
       <c r="L132" t="inlineStr"/>
       <c r="M132" t="inlineStr"/>
       <c r="N132" t="inlineStr"/>
@@ -11369,7 +11525,11 @@
       </c>
       <c r="I133" t="inlineStr"/>
       <c r="J133" t="inlineStr"/>
-      <c r="K133" t="inlineStr"/>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>prefer_oud_iop</t>
+        </is>
+      </c>
       <c r="L133" t="inlineStr"/>
       <c r="M133" t="inlineStr"/>
       <c r="N133" t="inlineStr"/>
@@ -11414,7 +11574,11 @@
       </c>
       <c r="I134" t="inlineStr"/>
       <c r="J134" t="inlineStr"/>
-      <c r="K134" t="inlineStr"/>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>prefer_oud_residential</t>
+        </is>
+      </c>
       <c r="L134" t="inlineStr"/>
       <c r="M134" t="inlineStr"/>
       <c r="N134" t="inlineStr"/>
@@ -11459,7 +11623,11 @@
       </c>
       <c r="I135" t="inlineStr"/>
       <c r="J135" t="inlineStr"/>
-      <c r="K135" t="inlineStr"/>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>prefer_oud_other_tx</t>
+        </is>
+      </c>
       <c r="L135" t="inlineStr"/>
       <c r="M135" t="inlineStr"/>
       <c r="N135" t="inlineStr"/>
@@ -11504,7 +11672,11 @@
       </c>
       <c r="I136" t="inlineStr"/>
       <c r="J136" t="inlineStr"/>
-      <c r="K136" t="inlineStr"/>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>prefer_oud_other_specify</t>
+        </is>
+      </c>
       <c r="L136" t="inlineStr"/>
       <c r="M136" t="inlineStr"/>
       <c r="N136" t="inlineStr"/>
@@ -11549,7 +11721,11 @@
       </c>
       <c r="I137" t="inlineStr"/>
       <c r="J137" t="inlineStr"/>
-      <c r="K137" t="inlineStr"/>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>prefer_oud_no_treatment</t>
+        </is>
+      </c>
       <c r="L137" t="inlineStr"/>
       <c r="M137" t="inlineStr"/>
       <c r="N137" t="inlineStr"/>
@@ -11594,7 +11770,11 @@
       </c>
       <c r="I138" t="inlineStr"/>
       <c r="J138" t="inlineStr"/>
-      <c r="K138" t="inlineStr"/>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>prefer_oud_dk</t>
+        </is>
+      </c>
       <c r="L138" t="inlineStr"/>
       <c r="M138" t="inlineStr"/>
       <c r="N138" t="inlineStr"/>
@@ -11635,7 +11815,11 @@
       </c>
       <c r="I139" t="inlineStr"/>
       <c r="J139" t="inlineStr"/>
-      <c r="K139" t="inlineStr"/>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>prefer_moud_type</t>
+        </is>
+      </c>
       <c r="L139" t="inlineStr"/>
       <c r="M139" t="inlineStr"/>
       <c r="N139" t="inlineStr"/>
@@ -11676,7 +11860,11 @@
       </c>
       <c r="I140" t="inlineStr"/>
       <c r="J140" t="inlineStr"/>
-      <c r="K140" t="inlineStr"/>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>prefer_which_bup</t>
+        </is>
+      </c>
       <c r="L140" t="inlineStr"/>
       <c r="M140" t="inlineStr"/>
       <c r="N140" t="inlineStr"/>
@@ -11717,7 +11905,11 @@
       </c>
       <c r="I141" t="inlineStr"/>
       <c r="J141" t="inlineStr"/>
-      <c r="K141" t="inlineStr"/>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>prefer_which_naloxone</t>
+        </is>
+      </c>
       <c r="L141" t="inlineStr"/>
       <c r="M141" t="inlineStr"/>
       <c r="N141" t="inlineStr"/>
@@ -11754,7 +11946,11 @@
       </c>
       <c r="I142" t="inlineStr"/>
       <c r="J142" t="inlineStr"/>
-      <c r="K142" t="inlineStr"/>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>household_people</t>
+        </is>
+      </c>
       <c r="L142" t="inlineStr"/>
       <c r="M142" t="inlineStr"/>
       <c r="N142" t="inlineStr">
@@ -11795,7 +11991,11 @@
       </c>
       <c r="I143" t="inlineStr"/>
       <c r="J143" t="inlineStr"/>
-      <c r="K143" t="inlineStr"/>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>household_under_18</t>
+        </is>
+      </c>
       <c r="L143" t="inlineStr"/>
       <c r="M143" t="inlineStr"/>
       <c r="N143" t="inlineStr">
@@ -11836,7 +12036,11 @@
       </c>
       <c r="I144" t="inlineStr"/>
       <c r="J144" t="inlineStr"/>
-      <c r="K144" t="inlineStr"/>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>household_income</t>
+        </is>
+      </c>
       <c r="L144" t="inlineStr"/>
       <c r="M144" t="inlineStr"/>
       <c r="N144" t="inlineStr">
@@ -11881,7 +12085,11 @@
       </c>
       <c r="I145" t="inlineStr"/>
       <c r="J145" t="inlineStr"/>
-      <c r="K145" t="inlineStr"/>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>household_income_legal</t>
+        </is>
+      </c>
       <c r="L145" t="inlineStr"/>
       <c r="M145" t="inlineStr"/>
       <c r="N145" t="inlineStr">
@@ -11930,7 +12138,11 @@
       </c>
       <c r="I146" t="inlineStr"/>
       <c r="J146" t="inlineStr"/>
-      <c r="K146" t="inlineStr"/>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>household_public_assist_any</t>
+        </is>
+      </c>
       <c r="L146" t="inlineStr"/>
       <c r="M146" t="inlineStr"/>
       <c r="N146" t="inlineStr">
@@ -11971,7 +12183,11 @@
       </c>
       <c r="I147" t="inlineStr"/>
       <c r="J147" t="inlineStr"/>
-      <c r="K147" t="inlineStr"/>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>household_public_assist_dollars</t>
+        </is>
+      </c>
       <c r="L147" t="inlineStr"/>
       <c r="M147" t="inlineStr"/>
       <c r="N147" t="inlineStr">
@@ -12012,7 +12228,11 @@
       </c>
       <c r="I148" t="inlineStr"/>
       <c r="J148" t="inlineStr"/>
-      <c r="K148" t="inlineStr"/>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>household_nonemploy_any</t>
+        </is>
+      </c>
       <c r="L148" t="inlineStr"/>
       <c r="M148" t="inlineStr"/>
       <c r="N148" t="inlineStr">
@@ -12053,7 +12273,11 @@
       </c>
       <c r="I149" t="inlineStr"/>
       <c r="J149" t="inlineStr"/>
-      <c r="K149" t="inlineStr"/>
+      <c r="K149" t="inlineStr">
+        <is>
+          <t>household_nonemploy_dollars</t>
+        </is>
+      </c>
       <c r="L149" t="inlineStr"/>
       <c r="M149" t="inlineStr"/>
       <c r="N149" t="inlineStr">
@@ -12102,7 +12326,11 @@
       </c>
       <c r="I150" t="inlineStr"/>
       <c r="J150" t="inlineStr"/>
-      <c r="K150" t="inlineStr"/>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>household_income_illegal_any</t>
+        </is>
+      </c>
       <c r="L150" t="inlineStr"/>
       <c r="M150" t="inlineStr"/>
       <c r="N150" t="inlineStr">
@@ -12143,7 +12371,11 @@
       </c>
       <c r="I151" t="inlineStr"/>
       <c r="J151" t="inlineStr"/>
-      <c r="K151" t="inlineStr"/>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>household_income_illegal_dollars</t>
+        </is>
+      </c>
       <c r="L151" t="inlineStr"/>
       <c r="M151" t="inlineStr"/>
       <c r="N151" t="inlineStr">
@@ -12188,7 +12420,11 @@
       </c>
       <c r="I152" t="inlineStr"/>
       <c r="J152" t="inlineStr"/>
-      <c r="K152" t="inlineStr"/>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>current_work_school</t>
+        </is>
+      </c>
       <c r="L152" t="inlineStr"/>
       <c r="M152" t="inlineStr"/>
       <c r="N152" t="inlineStr">
@@ -12229,7 +12465,11 @@
       </c>
       <c r="I153" t="inlineStr"/>
       <c r="J153" t="inlineStr"/>
-      <c r="K153" t="inlineStr"/>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>work_days</t>
+        </is>
+      </c>
       <c r="L153" t="inlineStr"/>
       <c r="M153" t="inlineStr"/>
       <c r="N153" t="inlineStr">
@@ -12270,7 +12510,11 @@
       </c>
       <c r="I154" t="inlineStr"/>
       <c r="J154" t="inlineStr"/>
-      <c r="K154" t="inlineStr"/>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>work_typical_days_week</t>
+        </is>
+      </c>
       <c r="L154" t="inlineStr"/>
       <c r="M154" t="inlineStr"/>
       <c r="N154" t="inlineStr">
@@ -12311,7 +12555,11 @@
       </c>
       <c r="I155" t="inlineStr"/>
       <c r="J155" t="inlineStr"/>
-      <c r="K155" t="inlineStr"/>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>work_hours_week</t>
+        </is>
+      </c>
       <c r="L155" t="inlineStr"/>
       <c r="M155" t="inlineStr"/>
       <c r="N155" t="inlineStr">
@@ -12352,7 +12600,11 @@
       </c>
       <c r="I156" t="inlineStr"/>
       <c r="J156" t="inlineStr"/>
-      <c r="K156" t="inlineStr"/>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>work_hourly_wage</t>
+        </is>
+      </c>
       <c r="L156" t="inlineStr"/>
       <c r="M156" t="inlineStr"/>
       <c r="N156" t="inlineStr">
@@ -12401,7 +12653,11 @@
       </c>
       <c r="I157" t="inlineStr"/>
       <c r="J157" t="inlineStr"/>
-      <c r="K157" t="inlineStr"/>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>work_health_insurance</t>
+        </is>
+      </c>
       <c r="L157" t="inlineStr"/>
       <c r="M157" t="inlineStr"/>
       <c r="N157" t="inlineStr">
@@ -12450,7 +12706,11 @@
       </c>
       <c r="I158" t="inlineStr"/>
       <c r="J158" t="inlineStr"/>
-      <c r="K158" t="inlineStr"/>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>work_paid_time_off</t>
+        </is>
+      </c>
       <c r="L158" t="inlineStr"/>
       <c r="M158" t="inlineStr"/>
       <c r="N158" t="inlineStr">
@@ -12499,7 +12759,11 @@
       </c>
       <c r="I159" t="inlineStr"/>
       <c r="J159" t="inlineStr"/>
-      <c r="K159" t="inlineStr"/>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>work_pension</t>
+        </is>
+      </c>
       <c r="L159" t="inlineStr"/>
       <c r="M159" t="inlineStr"/>
       <c r="N159" t="inlineStr">
@@ -12548,7 +12812,11 @@
       </c>
       <c r="I160" t="inlineStr"/>
       <c r="J160" t="inlineStr"/>
-      <c r="K160" t="inlineStr"/>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>work_retirement_plan</t>
+        </is>
+      </c>
       <c r="L160" t="inlineStr"/>
       <c r="M160" t="inlineStr"/>
       <c r="N160" t="inlineStr">
@@ -12589,7 +12857,11 @@
       </c>
       <c r="I161" t="inlineStr"/>
       <c r="J161" t="inlineStr"/>
-      <c r="K161" t="inlineStr"/>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>work_occupation</t>
+        </is>
+      </c>
       <c r="L161" t="inlineStr"/>
       <c r="M161" t="inlineStr"/>
       <c r="N161" t="inlineStr">
@@ -12638,7 +12910,11 @@
       </c>
       <c r="I162" t="inlineStr"/>
       <c r="J162" t="inlineStr"/>
-      <c r="K162" t="inlineStr"/>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>have_health_insurance</t>
+        </is>
+      </c>
       <c r="L162" t="inlineStr"/>
       <c r="M162" t="inlineStr"/>
       <c r="N162" t="inlineStr">
@@ -12687,7 +12963,11 @@
       </c>
       <c r="I163" t="inlineStr"/>
       <c r="J163" t="inlineStr"/>
-      <c r="K163" t="inlineStr"/>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>insured_private</t>
+        </is>
+      </c>
       <c r="L163" t="inlineStr"/>
       <c r="M163" t="inlineStr"/>
       <c r="N163" t="inlineStr">
@@ -12736,7 +13016,11 @@
       </c>
       <c r="I164" t="inlineStr"/>
       <c r="J164" t="inlineStr"/>
-      <c r="K164" t="inlineStr"/>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>insured_medicare</t>
+        </is>
+      </c>
       <c r="L164" t="inlineStr"/>
       <c r="M164" t="inlineStr"/>
       <c r="N164" t="inlineStr">
@@ -12785,7 +13069,11 @@
       </c>
       <c r="I165" t="inlineStr"/>
       <c r="J165" t="inlineStr"/>
-      <c r="K165" t="inlineStr"/>
+      <c r="K165" t="inlineStr">
+        <is>
+          <t>insured_medigap</t>
+        </is>
+      </c>
       <c r="L165" t="inlineStr"/>
       <c r="M165" t="inlineStr"/>
       <c r="N165" t="inlineStr">
@@ -12834,7 +13122,11 @@
       </c>
       <c r="I166" t="inlineStr"/>
       <c r="J166" t="inlineStr"/>
-      <c r="K166" t="inlineStr"/>
+      <c r="K166" t="inlineStr">
+        <is>
+          <t>insured_medicaid</t>
+        </is>
+      </c>
       <c r="L166" t="inlineStr"/>
       <c r="M166" t="inlineStr"/>
       <c r="N166" t="inlineStr">
@@ -12883,7 +13175,11 @@
       </c>
       <c r="I167" t="inlineStr"/>
       <c r="J167" t="inlineStr"/>
-      <c r="K167" t="inlineStr"/>
+      <c r="K167" t="inlineStr">
+        <is>
+          <t>insured_chip</t>
+        </is>
+      </c>
       <c r="L167" t="inlineStr"/>
       <c r="M167" t="inlineStr"/>
       <c r="N167" t="inlineStr">
@@ -12932,7 +13228,11 @@
       </c>
       <c r="I168" t="inlineStr"/>
       <c r="J168" t="inlineStr"/>
-      <c r="K168" t="inlineStr"/>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>insured_military</t>
+        </is>
+      </c>
       <c r="L168" t="inlineStr"/>
       <c r="M168" t="inlineStr"/>
       <c r="N168" t="inlineStr">
@@ -12981,7 +13281,11 @@
       </c>
       <c r="I169" t="inlineStr"/>
       <c r="J169" t="inlineStr"/>
-      <c r="K169" t="inlineStr"/>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>insured_indian</t>
+        </is>
+      </c>
       <c r="L169" t="inlineStr"/>
       <c r="M169" t="inlineStr"/>
       <c r="N169" t="inlineStr">
@@ -13030,7 +13334,11 @@
       </c>
       <c r="I170" t="inlineStr"/>
       <c r="J170" t="inlineStr"/>
-      <c r="K170" t="inlineStr"/>
+      <c r="K170" t="inlineStr">
+        <is>
+          <t>insured_state</t>
+        </is>
+      </c>
       <c r="L170" t="inlineStr"/>
       <c r="M170" t="inlineStr"/>
       <c r="N170" t="inlineStr">
@@ -13079,7 +13387,11 @@
       </c>
       <c r="I171" t="inlineStr"/>
       <c r="J171" t="inlineStr"/>
-      <c r="K171" t="inlineStr"/>
+      <c r="K171" t="inlineStr">
+        <is>
+          <t>insured_other_gov</t>
+        </is>
+      </c>
       <c r="L171" t="inlineStr"/>
       <c r="M171" t="inlineStr"/>
       <c r="N171" t="inlineStr">
@@ -13128,7 +13440,11 @@
       </c>
       <c r="I172" t="inlineStr"/>
       <c r="J172" t="inlineStr"/>
-      <c r="K172" t="inlineStr"/>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>insured_single_service</t>
+        </is>
+      </c>
       <c r="L172" t="inlineStr"/>
       <c r="M172" t="inlineStr"/>
       <c r="N172" t="inlineStr">
@@ -13177,7 +13493,11 @@
       </c>
       <c r="I173" t="inlineStr"/>
       <c r="J173" t="inlineStr"/>
-      <c r="K173" t="inlineStr"/>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>insured_dont_know</t>
+        </is>
+      </c>
       <c r="L173" t="inlineStr"/>
       <c r="M173" t="inlineStr"/>
       <c r="N173" t="inlineStr">
@@ -13218,7 +13538,11 @@
       </c>
       <c r="I174" t="inlineStr"/>
       <c r="J174" t="inlineStr"/>
-      <c r="K174" t="inlineStr"/>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>days_uninsured</t>
+        </is>
+      </c>
       <c r="L174" t="inlineStr"/>
       <c r="M174" t="inlineStr"/>
       <c r="N174" t="inlineStr">
@@ -13259,7 +13583,11 @@
       </c>
       <c r="I175" t="inlineStr"/>
       <c r="J175" t="inlineStr"/>
-      <c r="K175" t="inlineStr"/>
+      <c r="K175" t="inlineStr">
+        <is>
+          <t>days_self_help</t>
+        </is>
+      </c>
       <c r="L175" t="inlineStr"/>
       <c r="M175" t="inlineStr"/>
       <c r="N175" t="inlineStr">
@@ -13300,7 +13628,11 @@
       </c>
       <c r="I176" t="inlineStr"/>
       <c r="J176" t="inlineStr"/>
-      <c r="K176" t="inlineStr"/>
+      <c r="K176" t="inlineStr">
+        <is>
+          <t>days_drugfree_activity</t>
+        </is>
+      </c>
       <c r="L176" t="inlineStr"/>
       <c r="M176" t="inlineStr"/>
       <c r="N176" t="inlineStr">
@@ -13341,7 +13673,11 @@
       </c>
       <c r="I177" t="inlineStr"/>
       <c r="J177" t="inlineStr"/>
-      <c r="K177" t="inlineStr"/>
+      <c r="K177" t="inlineStr">
+        <is>
+          <t>days_homeless</t>
+        </is>
+      </c>
       <c r="L177" t="inlineStr"/>
       <c r="M177" t="inlineStr"/>
       <c r="N177" t="inlineStr">
@@ -13382,7 +13718,11 @@
       </c>
       <c r="I178" t="inlineStr"/>
       <c r="J178" t="inlineStr"/>
-      <c r="K178" t="inlineStr"/>
+      <c r="K178" t="inlineStr">
+        <is>
+          <t>days_shelter</t>
+        </is>
+      </c>
       <c r="L178" t="inlineStr"/>
       <c r="M178" t="inlineStr"/>
       <c r="N178" t="inlineStr">
@@ -13423,7 +13763,11 @@
       </c>
       <c r="I179" t="inlineStr"/>
       <c r="J179" t="inlineStr"/>
-      <c r="K179" t="inlineStr"/>
+      <c r="K179" t="inlineStr">
+        <is>
+          <t>days_household_alcohol</t>
+        </is>
+      </c>
       <c r="L179" t="inlineStr"/>
       <c r="M179" t="inlineStr"/>
       <c r="N179" t="inlineStr">
@@ -13464,7 +13808,11 @@
       </c>
       <c r="I180" t="inlineStr"/>
       <c r="J180" t="inlineStr"/>
-      <c r="K180" t="inlineStr"/>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>days_household_drug</t>
+        </is>
+      </c>
       <c r="L180" t="inlineStr"/>
       <c r="M180" t="inlineStr"/>
       <c r="N180" t="inlineStr">
@@ -13505,7 +13853,11 @@
       </c>
       <c r="I181" t="inlineStr"/>
       <c r="J181" t="inlineStr"/>
-      <c r="K181" t="inlineStr"/>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>days_activities_substance_use</t>
+        </is>
+      </c>
       <c r="L181" t="inlineStr"/>
       <c r="M181" t="inlineStr"/>
       <c r="N181" t="inlineStr">
@@ -13546,7 +13898,11 @@
       </c>
       <c r="I182" t="inlineStr"/>
       <c r="J182" t="inlineStr"/>
-      <c r="K182" t="inlineStr"/>
+      <c r="K182" t="inlineStr">
+        <is>
+          <t>days_family_trouble</t>
+        </is>
+      </c>
       <c r="L182" t="inlineStr"/>
       <c r="M182" t="inlineStr"/>
       <c r="N182" t="inlineStr">
@@ -13587,7 +13943,11 @@
       </c>
       <c r="I183" t="inlineStr"/>
       <c r="J183" t="inlineStr"/>
-      <c r="K183" t="inlineStr"/>
+      <c r="K183" t="inlineStr">
+        <is>
+          <t>days_arguments</t>
+        </is>
+      </c>
       <c r="L183" t="inlineStr"/>
       <c r="M183" t="inlineStr"/>
       <c r="N183" t="inlineStr">
@@ -13628,7 +13988,11 @@
       </c>
       <c r="I184" t="inlineStr"/>
       <c r="J184" t="inlineStr"/>
-      <c r="K184" t="inlineStr"/>
+      <c r="K184" t="inlineStr">
+        <is>
+          <t>days_abused</t>
+        </is>
+      </c>
       <c r="L184" t="inlineStr"/>
       <c r="M184" t="inlineStr"/>
       <c r="N184" t="inlineStr">
@@ -13677,7 +14041,11 @@
       </c>
       <c r="I185" t="inlineStr"/>
       <c r="J185" t="inlineStr"/>
-      <c r="K185" t="inlineStr"/>
+      <c r="K185" t="inlineStr">
+        <is>
+          <t>narcan_received</t>
+        </is>
+      </c>
       <c r="L185" t="inlineStr"/>
       <c r="M185" t="inlineStr"/>
       <c r="N185" t="inlineStr">
@@ -13726,7 +14094,11 @@
       </c>
       <c r="I186" t="inlineStr"/>
       <c r="J186" t="inlineStr"/>
-      <c r="K186" t="inlineStr"/>
+      <c r="K186" t="inlineStr">
+        <is>
+          <t>narcan_used</t>
+        </is>
+      </c>
       <c r="L186" t="inlineStr"/>
       <c r="M186" t="inlineStr"/>
       <c r="N186" t="inlineStr">
@@ -13775,7 +14147,11 @@
       </c>
       <c r="I187" t="inlineStr"/>
       <c r="J187" t="inlineStr"/>
-      <c r="K187" t="inlineStr"/>
+      <c r="K187" t="inlineStr">
+        <is>
+          <t>narcan_refilled</t>
+        </is>
+      </c>
       <c r="L187" t="inlineStr"/>
       <c r="M187" t="inlineStr"/>
       <c r="N187" t="inlineStr">
@@ -13820,7 +14196,11 @@
       </c>
       <c r="I188" t="inlineStr"/>
       <c r="J188" t="inlineStr"/>
-      <c r="K188" t="inlineStr"/>
+      <c r="K188" t="inlineStr">
+        <is>
+          <t>difficulty_chores</t>
+        </is>
+      </c>
       <c r="L188" t="inlineStr"/>
       <c r="M188" t="inlineStr"/>
       <c r="N188" t="inlineStr"/>
@@ -13861,7 +14241,11 @@
       </c>
       <c r="I189" t="inlineStr"/>
       <c r="J189" t="inlineStr"/>
-      <c r="K189" t="inlineStr"/>
+      <c r="K189" t="inlineStr">
+        <is>
+          <t>difficulty_stairs</t>
+        </is>
+      </c>
       <c r="L189" t="inlineStr"/>
       <c r="M189" t="inlineStr"/>
       <c r="N189" t="inlineStr"/>
@@ -13902,7 +14286,11 @@
       </c>
       <c r="I190" t="inlineStr"/>
       <c r="J190" t="inlineStr"/>
-      <c r="K190" t="inlineStr"/>
+      <c r="K190" t="inlineStr">
+        <is>
+          <t>difficulty_walking</t>
+        </is>
+      </c>
       <c r="L190" t="inlineStr"/>
       <c r="M190" t="inlineStr"/>
       <c r="N190" t="inlineStr"/>
@@ -13943,7 +14331,11 @@
       </c>
       <c r="I191" t="inlineStr"/>
       <c r="J191" t="inlineStr"/>
-      <c r="K191" t="inlineStr"/>
+      <c r="K191" t="inlineStr">
+        <is>
+          <t>difficulty_traveling</t>
+        </is>
+      </c>
       <c r="L191" t="inlineStr"/>
       <c r="M191" t="inlineStr"/>
       <c r="N191" t="inlineStr"/>
@@ -13984,7 +14376,11 @@
       </c>
       <c r="I192" t="inlineStr"/>
       <c r="J192" t="inlineStr"/>
-      <c r="K192" t="inlineStr"/>
+      <c r="K192" t="inlineStr">
+        <is>
+          <t>trouble_with_leisure</t>
+        </is>
+      </c>
       <c r="L192" t="inlineStr"/>
       <c r="M192" t="inlineStr"/>
       <c r="N192" t="inlineStr"/>
@@ -14025,7 +14421,11 @@
       </c>
       <c r="I193" t="inlineStr"/>
       <c r="J193" t="inlineStr"/>
-      <c r="K193" t="inlineStr"/>
+      <c r="K193" t="inlineStr">
+        <is>
+          <t>trouble_with_family</t>
+        </is>
+      </c>
       <c r="L193" t="inlineStr"/>
       <c r="M193" t="inlineStr"/>
       <c r="N193" t="inlineStr"/>
@@ -14066,7 +14466,11 @@
       </c>
       <c r="I194" t="inlineStr"/>
       <c r="J194" t="inlineStr"/>
-      <c r="K194" t="inlineStr"/>
+      <c r="K194" t="inlineStr">
+        <is>
+          <t>trouble_with_work</t>
+        </is>
+      </c>
       <c r="L194" t="inlineStr"/>
       <c r="M194" t="inlineStr"/>
       <c r="N194" t="inlineStr"/>
@@ -14107,7 +14511,11 @@
       </c>
       <c r="I195" t="inlineStr"/>
       <c r="J195" t="inlineStr"/>
-      <c r="K195" t="inlineStr"/>
+      <c r="K195" t="inlineStr">
+        <is>
+          <t>trouble_with_activities</t>
+        </is>
+      </c>
       <c r="L195" t="inlineStr"/>
       <c r="M195" t="inlineStr"/>
       <c r="N195" t="inlineStr"/>
@@ -14148,7 +14556,11 @@
       </c>
       <c r="I196" t="inlineStr"/>
       <c r="J196" t="inlineStr"/>
-      <c r="K196" t="inlineStr"/>
+      <c r="K196" t="inlineStr">
+        <is>
+          <t>past_week_fearful</t>
+        </is>
+      </c>
       <c r="L196" t="inlineStr"/>
       <c r="M196" t="inlineStr"/>
       <c r="N196" t="inlineStr"/>
@@ -14189,7 +14601,11 @@
       </c>
       <c r="I197" t="inlineStr"/>
       <c r="J197" t="inlineStr"/>
-      <c r="K197" t="inlineStr"/>
+      <c r="K197" t="inlineStr">
+        <is>
+          <t>past_week_anxiety</t>
+        </is>
+      </c>
       <c r="L197" t="inlineStr"/>
       <c r="M197" t="inlineStr"/>
       <c r="N197" t="inlineStr"/>
@@ -14230,7 +14646,11 @@
       </c>
       <c r="I198" t="inlineStr"/>
       <c r="J198" t="inlineStr"/>
-      <c r="K198" t="inlineStr"/>
+      <c r="K198" t="inlineStr">
+        <is>
+          <t>past_week_worried</t>
+        </is>
+      </c>
       <c r="L198" t="inlineStr"/>
       <c r="M198" t="inlineStr"/>
       <c r="N198" t="inlineStr"/>
@@ -14271,7 +14691,11 @@
       </c>
       <c r="I199" t="inlineStr"/>
       <c r="J199" t="inlineStr"/>
-      <c r="K199" t="inlineStr"/>
+      <c r="K199" t="inlineStr">
+        <is>
+          <t>past_week_uneasy</t>
+        </is>
+      </c>
       <c r="L199" t="inlineStr"/>
       <c r="M199" t="inlineStr"/>
       <c r="N199" t="inlineStr"/>
@@ -14312,7 +14736,11 @@
       </c>
       <c r="I200" t="inlineStr"/>
       <c r="J200" t="inlineStr"/>
-      <c r="K200" t="inlineStr"/>
+      <c r="K200" t="inlineStr">
+        <is>
+          <t>past_week_worthless</t>
+        </is>
+      </c>
       <c r="L200" t="inlineStr"/>
       <c r="M200" t="inlineStr"/>
       <c r="N200" t="inlineStr"/>
@@ -14353,7 +14781,11 @@
       </c>
       <c r="I201" t="inlineStr"/>
       <c r="J201" t="inlineStr"/>
-      <c r="K201" t="inlineStr"/>
+      <c r="K201" t="inlineStr">
+        <is>
+          <t>past_week_helpless</t>
+        </is>
+      </c>
       <c r="L201" t="inlineStr"/>
       <c r="M201" t="inlineStr"/>
       <c r="N201" t="inlineStr"/>
@@ -14394,7 +14826,11 @@
       </c>
       <c r="I202" t="inlineStr"/>
       <c r="J202" t="inlineStr"/>
-      <c r="K202" t="inlineStr"/>
+      <c r="K202" t="inlineStr">
+        <is>
+          <t>past_week_depressed</t>
+        </is>
+      </c>
       <c r="L202" t="inlineStr"/>
       <c r="M202" t="inlineStr"/>
       <c r="N202" t="inlineStr"/>
@@ -14435,7 +14871,11 @@
       </c>
       <c r="I203" t="inlineStr"/>
       <c r="J203" t="inlineStr"/>
-      <c r="K203" t="inlineStr"/>
+      <c r="K203" t="inlineStr">
+        <is>
+          <t>past_week_hopeless</t>
+        </is>
+      </c>
       <c r="L203" t="inlineStr"/>
       <c r="M203" t="inlineStr"/>
       <c r="N203" t="inlineStr"/>
@@ -14476,7 +14916,11 @@
       </c>
       <c r="I204" t="inlineStr"/>
       <c r="J204" t="inlineStr"/>
-      <c r="K204" t="inlineStr"/>
+      <c r="K204" t="inlineStr">
+        <is>
+          <t>past_week_fatigued</t>
+        </is>
+      </c>
       <c r="L204" t="inlineStr"/>
       <c r="M204" t="inlineStr"/>
       <c r="N204" t="inlineStr"/>
@@ -14517,7 +14961,11 @@
       </c>
       <c r="I205" t="inlineStr"/>
       <c r="J205" t="inlineStr"/>
-      <c r="K205" t="inlineStr"/>
+      <c r="K205" t="inlineStr">
+        <is>
+          <t>past_week_tired</t>
+        </is>
+      </c>
       <c r="L205" t="inlineStr"/>
       <c r="M205" t="inlineStr"/>
       <c r="N205" t="inlineStr"/>
@@ -14558,7 +15006,11 @@
       </c>
       <c r="I206" t="inlineStr"/>
       <c r="J206" t="inlineStr"/>
-      <c r="K206" t="inlineStr"/>
+      <c r="K206" t="inlineStr">
+        <is>
+          <t>past_week_rundown</t>
+        </is>
+      </c>
       <c r="L206" t="inlineStr"/>
       <c r="M206" t="inlineStr"/>
       <c r="N206" t="inlineStr"/>
@@ -14599,7 +15051,11 @@
       </c>
       <c r="I207" t="inlineStr"/>
       <c r="J207" t="inlineStr"/>
-      <c r="K207" t="inlineStr"/>
+      <c r="K207" t="inlineStr">
+        <is>
+          <t>fatigue_level</t>
+        </is>
+      </c>
       <c r="L207" t="inlineStr"/>
       <c r="M207" t="inlineStr"/>
       <c r="N207" t="inlineStr"/>
@@ -14640,7 +15096,11 @@
       </c>
       <c r="I208" t="inlineStr"/>
       <c r="J208" t="inlineStr"/>
-      <c r="K208" t="inlineStr"/>
+      <c r="K208" t="inlineStr">
+        <is>
+          <t>sleep_quality</t>
+        </is>
+      </c>
       <c r="L208" t="inlineStr"/>
       <c r="M208" t="inlineStr"/>
       <c r="N208" t="inlineStr"/>
@@ -14681,7 +15141,11 @@
       </c>
       <c r="I209" t="inlineStr"/>
       <c r="J209" t="inlineStr"/>
-      <c r="K209" t="inlineStr"/>
+      <c r="K209" t="inlineStr">
+        <is>
+          <t>sleep_refreshing</t>
+        </is>
+      </c>
       <c r="L209" t="inlineStr"/>
       <c r="M209" t="inlineStr"/>
       <c r="N209" t="inlineStr"/>
@@ -14722,7 +15186,11 @@
       </c>
       <c r="I210" t="inlineStr"/>
       <c r="J210" t="inlineStr"/>
-      <c r="K210" t="inlineStr"/>
+      <c r="K210" t="inlineStr">
+        <is>
+          <t>sleep_problems</t>
+        </is>
+      </c>
       <c r="L210" t="inlineStr"/>
       <c r="M210" t="inlineStr"/>
       <c r="N210" t="inlineStr"/>
@@ -14763,7 +15231,11 @@
       </c>
       <c r="I211" t="inlineStr"/>
       <c r="J211" t="inlineStr"/>
-      <c r="K211" t="inlineStr"/>
+      <c r="K211" t="inlineStr">
+        <is>
+          <t>sleep_difficulty</t>
+        </is>
+      </c>
       <c r="L211" t="inlineStr"/>
       <c r="M211" t="inlineStr"/>
       <c r="N211" t="inlineStr"/>
@@ -14804,7 +15276,11 @@
       </c>
       <c r="I212" t="inlineStr"/>
       <c r="J212" t="inlineStr"/>
-      <c r="K212" t="inlineStr"/>
+      <c r="K212" t="inlineStr">
+        <is>
+          <t>can_concentrate</t>
+        </is>
+      </c>
       <c r="L212" t="inlineStr"/>
       <c r="M212" t="inlineStr"/>
       <c r="N212" t="inlineStr"/>
@@ -14845,7 +15321,11 @@
       </c>
       <c r="I213" t="inlineStr"/>
       <c r="J213" t="inlineStr"/>
-      <c r="K213" t="inlineStr"/>
+      <c r="K213" t="inlineStr">
+        <is>
+          <t>can_remember</t>
+        </is>
+      </c>
       <c r="L213" t="inlineStr"/>
       <c r="M213" t="inlineStr"/>
       <c r="N213" t="inlineStr"/>
@@ -14886,7 +15366,11 @@
       </c>
       <c r="I214" t="inlineStr"/>
       <c r="J214" t="inlineStr"/>
-      <c r="K214" t="inlineStr"/>
+      <c r="K214" t="inlineStr">
+        <is>
+          <t>pain_daily_activity</t>
+        </is>
+      </c>
       <c r="L214" t="inlineStr"/>
       <c r="M214" t="inlineStr"/>
       <c r="N214" t="inlineStr"/>
@@ -14927,7 +15411,11 @@
       </c>
       <c r="I215" t="inlineStr"/>
       <c r="J215" t="inlineStr"/>
-      <c r="K215" t="inlineStr"/>
+      <c r="K215" t="inlineStr">
+        <is>
+          <t>pain_work_around_house</t>
+        </is>
+      </c>
       <c r="L215" t="inlineStr"/>
       <c r="M215" t="inlineStr"/>
       <c r="N215" t="inlineStr"/>
@@ -14968,7 +15456,11 @@
       </c>
       <c r="I216" t="inlineStr"/>
       <c r="J216" t="inlineStr"/>
-      <c r="K216" t="inlineStr"/>
+      <c r="K216" t="inlineStr">
+        <is>
+          <t>pain_social_activity</t>
+        </is>
+      </c>
       <c r="L216" t="inlineStr"/>
       <c r="M216" t="inlineStr"/>
       <c r="N216" t="inlineStr"/>
@@ -15009,7 +15501,11 @@
       </c>
       <c r="I217" t="inlineStr"/>
       <c r="J217" t="inlineStr"/>
-      <c r="K217" t="inlineStr"/>
+      <c r="K217" t="inlineStr">
+        <is>
+          <t>pain_household_chores</t>
+        </is>
+      </c>
       <c r="L217" t="inlineStr"/>
       <c r="M217" t="inlineStr"/>
       <c r="N217" t="inlineStr"/>
@@ -15046,7 +15542,11 @@
       </c>
       <c r="I218" t="inlineStr"/>
       <c r="J218" t="inlineStr"/>
-      <c r="K218" t="inlineStr"/>
+      <c r="K218" t="inlineStr">
+        <is>
+          <t>pain_intensity</t>
+        </is>
+      </c>
       <c r="L218" t="inlineStr"/>
       <c r="M218" t="inlineStr"/>
       <c r="N218" t="inlineStr"/>
@@ -15089,7 +15589,11 @@
       </c>
       <c r="I219" t="inlineStr"/>
       <c r="J219" t="inlineStr"/>
-      <c r="K219" t="inlineStr"/>
+      <c r="K219" t="inlineStr">
+        <is>
+          <t>last_time_multiple_partners</t>
+        </is>
+      </c>
       <c r="L219" t="inlineStr"/>
       <c r="M219" t="inlineStr"/>
       <c r="N219" t="inlineStr">
@@ -15134,7 +15638,11 @@
       </c>
       <c r="I220" t="inlineStr"/>
       <c r="J220" t="inlineStr"/>
-      <c r="K220" t="inlineStr"/>
+      <c r="K220" t="inlineStr">
+        <is>
+          <t>last_time_unprotected_sex</t>
+        </is>
+      </c>
       <c r="L220" t="inlineStr"/>
       <c r="M220" t="inlineStr"/>
       <c r="N220" t="inlineStr">
@@ -15179,7 +15687,11 @@
       </c>
       <c r="I221" t="inlineStr"/>
       <c r="J221" t="inlineStr"/>
-      <c r="K221" t="inlineStr"/>
+      <c r="K221" t="inlineStr">
+        <is>
+          <t>last_time_sex_intoxicated</t>
+        </is>
+      </c>
       <c r="L221" t="inlineStr"/>
       <c r="M221" t="inlineStr"/>
       <c r="N221" t="inlineStr">
@@ -15224,7 +15736,11 @@
       </c>
       <c r="I222" t="inlineStr"/>
       <c r="J222" t="inlineStr"/>
-      <c r="K222" t="inlineStr"/>
+      <c r="K222" t="inlineStr">
+        <is>
+          <t>last_time_injection_drug</t>
+        </is>
+      </c>
       <c r="L222" t="inlineStr"/>
       <c r="M222" t="inlineStr"/>
       <c r="N222" t="inlineStr">
@@ -15269,7 +15785,11 @@
       </c>
       <c r="I223" t="inlineStr"/>
       <c r="J223" t="inlineStr"/>
-      <c r="K223" t="inlineStr"/>
+      <c r="K223" t="inlineStr">
+        <is>
+          <t>last_time_attacked_weapon</t>
+        </is>
+      </c>
       <c r="L223" t="inlineStr"/>
       <c r="M223" t="inlineStr"/>
       <c r="N223" t="inlineStr">
@@ -15314,7 +15834,11 @@
       </c>
       <c r="I224" t="inlineStr"/>
       <c r="J224" t="inlineStr"/>
-      <c r="K224" t="inlineStr"/>
+      <c r="K224" t="inlineStr">
+        <is>
+          <t>last_time_physical_abuse</t>
+        </is>
+      </c>
       <c r="L224" t="inlineStr"/>
       <c r="M224" t="inlineStr"/>
       <c r="N224" t="inlineStr">
@@ -15359,7 +15883,11 @@
       </c>
       <c r="I225" t="inlineStr"/>
       <c r="J225" t="inlineStr"/>
-      <c r="K225" t="inlineStr"/>
+      <c r="K225" t="inlineStr">
+        <is>
+          <t>last_time_sex_abuse</t>
+        </is>
+      </c>
       <c r="L225" t="inlineStr"/>
       <c r="M225" t="inlineStr"/>
       <c r="N225" t="inlineStr">
@@ -15404,7 +15932,11 @@
       </c>
       <c r="I226" t="inlineStr"/>
       <c r="J226" t="inlineStr"/>
-      <c r="K226" t="inlineStr"/>
+      <c r="K226" t="inlineStr">
+        <is>
+          <t>last_time_emotional_abuse</t>
+        </is>
+      </c>
       <c r="L226" t="inlineStr"/>
       <c r="M226" t="inlineStr"/>
       <c r="N226" t="inlineStr">
@@ -15449,7 +15981,11 @@
       </c>
       <c r="I227" t="inlineStr"/>
       <c r="J227" t="inlineStr"/>
-      <c r="K227" t="inlineStr"/>
+      <c r="K227" t="inlineStr">
+        <is>
+          <t>last_time_ongoing_abuse</t>
+        </is>
+      </c>
       <c r="L227" t="inlineStr"/>
       <c r="M227" t="inlineStr"/>
       <c r="N227" t="inlineStr">
@@ -15494,7 +16030,11 @@
       </c>
       <c r="I228" t="inlineStr"/>
       <c r="J228" t="inlineStr"/>
-      <c r="K228" t="inlineStr"/>
+      <c r="K228" t="inlineStr">
+        <is>
+          <t>last_time_afraid_abuse</t>
+        </is>
+      </c>
       <c r="L228" t="inlineStr"/>
       <c r="M228" t="inlineStr"/>
       <c r="N228" t="inlineStr">
@@ -15539,7 +16079,11 @@
       </c>
       <c r="I229" t="inlineStr"/>
       <c r="J229" t="inlineStr"/>
-      <c r="K229" t="inlineStr"/>
+      <c r="K229" t="inlineStr">
+        <is>
+          <t>last_time_distressed_past</t>
+        </is>
+      </c>
       <c r="L229" t="inlineStr"/>
       <c r="M229" t="inlineStr"/>
       <c r="N229" t="inlineStr">
@@ -15584,7 +16128,11 @@
       </c>
       <c r="I230" t="inlineStr"/>
       <c r="J230" t="inlineStr"/>
-      <c r="K230" t="inlineStr"/>
+      <c r="K230" t="inlineStr">
+        <is>
+          <t>last_time_suicidal</t>
+        </is>
+      </c>
       <c r="L230" t="inlineStr"/>
       <c r="M230" t="inlineStr"/>
       <c r="N230" t="inlineStr">
@@ -15633,7 +16181,11 @@
       </c>
       <c r="I231" t="inlineStr"/>
       <c r="J231" t="inlineStr"/>
-      <c r="K231" t="inlineStr"/>
+      <c r="K231" t="inlineStr">
+        <is>
+          <t>ever_dx_hiv</t>
+        </is>
+      </c>
       <c r="L231" t="inlineStr"/>
       <c r="M231" t="inlineStr"/>
       <c r="N231" t="inlineStr">
@@ -15682,7 +16234,11 @@
       </c>
       <c r="I232" t="inlineStr"/>
       <c r="J232" t="inlineStr"/>
-      <c r="K232" t="inlineStr"/>
+      <c r="K232" t="inlineStr">
+        <is>
+          <t>ever_dx_hcv</t>
+        </is>
+      </c>
       <c r="L232" t="inlineStr"/>
       <c r="M232" t="inlineStr"/>
       <c r="N232" t="inlineStr">
@@ -15731,7 +16287,11 @@
       </c>
       <c r="I233" t="inlineStr"/>
       <c r="J233" t="inlineStr"/>
-      <c r="K233" t="inlineStr"/>
+      <c r="K233" t="inlineStr">
+        <is>
+          <t>ever_dx_hepb</t>
+        </is>
+      </c>
       <c r="L233" t="inlineStr"/>
       <c r="M233" t="inlineStr"/>
       <c r="N233" t="inlineStr">
@@ -15780,7 +16340,11 @@
       </c>
       <c r="I234" t="inlineStr"/>
       <c r="J234" t="inlineStr"/>
-      <c r="K234" t="inlineStr"/>
+      <c r="K234" t="inlineStr">
+        <is>
+          <t>ever_dx_std</t>
+        </is>
+      </c>
       <c r="L234" t="inlineStr"/>
       <c r="M234" t="inlineStr"/>
       <c r="N234" t="inlineStr">
@@ -15829,7 +16393,11 @@
       </c>
       <c r="I235" t="inlineStr"/>
       <c r="J235" t="inlineStr"/>
-      <c r="K235" t="inlineStr"/>
+      <c r="K235" t="inlineStr">
+        <is>
+          <t>ever_dx_tb</t>
+        </is>
+      </c>
       <c r="L235" t="inlineStr"/>
       <c r="M235" t="inlineStr"/>
       <c r="N235" t="inlineStr">
@@ -15878,7 +16446,11 @@
       </c>
       <c r="I236" t="inlineStr"/>
       <c r="J236" t="inlineStr"/>
-      <c r="K236" t="inlineStr"/>
+      <c r="K236" t="inlineStr">
+        <is>
+          <t>ever_dx_covid</t>
+        </is>
+      </c>
       <c r="L236" t="inlineStr"/>
       <c r="M236" t="inlineStr"/>
       <c r="N236" t="inlineStr">
@@ -15923,7 +16495,11 @@
       </c>
       <c r="I237" t="inlineStr"/>
       <c r="J237" t="inlineStr"/>
-      <c r="K237" t="inlineStr"/>
+      <c r="K237" t="inlineStr">
+        <is>
+          <t>first_dx_hiv</t>
+        </is>
+      </c>
       <c r="L237" t="inlineStr"/>
       <c r="M237" t="inlineStr"/>
       <c r="N237" t="inlineStr">
@@ -15968,7 +16544,11 @@
       </c>
       <c r="I238" t="inlineStr"/>
       <c r="J238" t="inlineStr"/>
-      <c r="K238" t="inlineStr"/>
+      <c r="K238" t="inlineStr">
+        <is>
+          <t>first_dx_hcv</t>
+        </is>
+      </c>
       <c r="L238" t="inlineStr"/>
       <c r="M238" t="inlineStr"/>
       <c r="N238" t="inlineStr">
@@ -16013,7 +16593,11 @@
       </c>
       <c r="I239" t="inlineStr"/>
       <c r="J239" t="inlineStr"/>
-      <c r="K239" t="inlineStr"/>
+      <c r="K239" t="inlineStr">
+        <is>
+          <t>first_dx_hepb</t>
+        </is>
+      </c>
       <c r="L239" t="inlineStr"/>
       <c r="M239" t="inlineStr"/>
       <c r="N239" t="inlineStr">
@@ -16058,7 +16642,11 @@
       </c>
       <c r="I240" t="inlineStr"/>
       <c r="J240" t="inlineStr"/>
-      <c r="K240" t="inlineStr"/>
+      <c r="K240" t="inlineStr">
+        <is>
+          <t>first_dx_std</t>
+        </is>
+      </c>
       <c r="L240" t="inlineStr"/>
       <c r="M240" t="inlineStr"/>
       <c r="N240" t="inlineStr">
@@ -16103,7 +16691,11 @@
       </c>
       <c r="I241" t="inlineStr"/>
       <c r="J241" t="inlineStr"/>
-      <c r="K241" t="inlineStr"/>
+      <c r="K241" t="inlineStr">
+        <is>
+          <t>first_dx_tb</t>
+        </is>
+      </c>
       <c r="L241" t="inlineStr"/>
       <c r="M241" t="inlineStr"/>
       <c r="N241" t="inlineStr">
@@ -16148,7 +16740,11 @@
       </c>
       <c r="I242" t="inlineStr"/>
       <c r="J242" t="inlineStr"/>
-      <c r="K242" t="inlineStr"/>
+      <c r="K242" t="inlineStr">
+        <is>
+          <t>first_dx_covid</t>
+        </is>
+      </c>
       <c r="L242" t="inlineStr"/>
       <c r="M242" t="inlineStr"/>
       <c r="N242" t="inlineStr">

</xml_diff>

<commit_message>
moved jcoin namespace fields back under custom property
</commit_message>
<xml_diff>
--- a/xlsx/core_measures.xlsx
+++ b/xlsx/core_measures.xlsx
@@ -610,18 +610,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="26" customWidth="1" min="1" max="1"/>
-    <col width="24" customWidth="1" min="2" max="2"/>
-    <col width="10" customWidth="1" min="3" max="3"/>
-    <col width="76" customWidth="1" min="4" max="4"/>
-    <col width="10" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="164" customWidth="1" min="7" max="7"/>
-    <col width="36.5" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="21" customWidth="1" min="10" max="10"/>
-    <col width="41" customWidth="1" min="11" max="11"/>
-    <col width="26" customWidth="1" min="12" max="12"/>
+    <col width="24" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="76" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="11" customWidth="1" min="5" max="5"/>
+    <col width="164" customWidth="1" min="6" max="6"/>
+    <col width="33" customWidth="1" min="7" max="7"/>
+    <col width="32" customWidth="1" min="8" max="8"/>
+    <col width="36.5" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
+    <col width="41" customWidth="1" min="12" max="12"/>
     <col width="6" customWidth="1" min="13" max="13"/>
     <col width="171" customWidth="1" min="14" max="14"/>
   </cols>
@@ -629,64 +629,64 @@
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>jcoin:core_measure_section</t>
+          <t>name</t>
         </is>
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>type</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>type</t>
+          <t>description</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>trueValues</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>trueValues</t>
+          <t>falseValues</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>falseValues</t>
+          <t>constraints.enum</t>
         </is>
       </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>constraints.enum</t>
+          <t>custom.jcoin:core_measure_section</t>
         </is>
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
+          <t>custom.jcoin:final_variable_name</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t>constraints.required</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t>constraints.maxLength</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="L1" s="2" t="inlineStr">
         <is>
           <t>constraints.pattern</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
-        <is>
-          <t>jcoin:final_variable_name</t>
-        </is>
-      </c>
       <c r="M1" s="2" t="inlineStr">
         <is>
           <t>format</t>
@@ -694,53 +694,53 @@
       </c>
       <c r="N1" s="2" t="inlineStr">
         <is>
-          <t>jcoin:notes</t>
+          <t>custom.jcoin:notes</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Record and linkage</t>
+          <t>jdc_person_id</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>jdc_person_id</t>
+          <t>string</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
           <t>The generated unique identifier specific to the JCOIN Data Commons for a given individual (client or staff).</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Record and linkage</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>jdc_person_id</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>JCOIN data commons person identifier</t>
         </is>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>1</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>9</v>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>[A-Z][0-9][0-9][0-9]-[0-9][0-9][0-9][0-9]</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>jdc_person_id</t>
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
@@ -749,46 +749,46 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Enrollment</t>
+          <t>quarter_enrolled</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>quarter_enrolled</t>
+          <t>string</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
           <t>The financial quarter and year of enrollment</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Enrollment</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
+          <t>quarter_enrolled</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
           <t>Quarter Enrolled</t>
         </is>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>1</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>6</v>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>[0-9][0-9][0-9][0-9]Q[0-9]</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>quarter_enrolled</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
@@ -797,46 +797,46 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Enrollment</t>
+          <t>state_of_site_enrollment</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>state_of_site_enrollment</t>
+          <t>string</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
           <t>The U.S. State abbreviation of the site where client (participant) was initially enrolled</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Enrollment</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr">
         <is>
+          <t>state_of_site_enrollment</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
           <t>State of Site For Enrollment</t>
         </is>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>1</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>2</v>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>[A-Z][A-Z]</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>state_of_site_enrollment</t>
         </is>
       </c>
       <c r="M4" t="inlineStr"/>
@@ -845,86 +845,86 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>current_study_status</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>A summary of the current status where client (participant) is in study</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>On study|Dropped out|Withdrawn by investigator|Completed study|Unknown</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>Enrollment</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>current_study_status</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>A summary of the current status where client (participant) is in study</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>On study|Dropped out|Withdrawn by investigator|Completed study|Unknown</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Current Study Status</t>
         </is>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>1</v>
       </c>
-      <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>current_study_status</t>
-        </is>
-      </c>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Demographics</t>
+          <t>d1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>d1</t>
+          <t>date</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
           <t>What is your birth date?</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Demographics</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
+          <t>birth_date</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
           <t>Birth date</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>birth_date</t>
-        </is>
-      </c>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr">
         <is>
           <t>%Y%m%d</t>
@@ -935,128 +935,128 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Demographics</t>
+          <t>d1a</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>d1a</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>integer</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
           <t>About how old are you? (top coded at 90)</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Demographics</t>
+        </is>
+      </c>
       <c r="H7" t="inlineStr">
         <is>
+          <t>age</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
           <t>Age</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>age</t>
-        </is>
-      </c>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>o1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>What sex was originally listed on your birth certificate?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Male|Female|Decline to answer|Something else</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>o1</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>What sex was originally listed on your birth certificate?</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Male|Female|Decline to answer|Something else</t>
-        </is>
-      </c>
       <c r="H8" t="inlineStr">
         <is>
+          <t>sex_at_birth</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
           <t>Sex at birth</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>sex_at_birth</t>
-        </is>
-      </c>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>o2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>What is your gender identity?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Male|Female|Transgender man/trans man/female-to-male (FTM)|Transgender woman/trans woman/male-to-female (MTF)|Genderqueer/gender nonconforming/neither exclusively male nor female|Additional gender category (or other)|Not reported</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>o2</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>What is your gender identity?</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Male|Female|Transgender man/trans man/female-to-male (FTM)|Transgender woman/trans woman/male-to-female (MTF)|Genderqueer/gender nonconforming/neither exclusively male nor female|Additional gender category (or other)|Not reported</t>
-        </is>
-      </c>
       <c r="H9" t="inlineStr">
         <is>
+          <t>gender_id</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
           <t>Gender Identity</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>gender_id</t>
-        </is>
-      </c>
+      <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr">
         <is>
@@ -1068,44 +1068,44 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>d4b</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>What is your gender identity?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Male|Female|Transgender|Gender nonconforming|Something else|Not reported</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>d4b</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>What is your gender identity?</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Male|Female|Transgender|Gender nonconforming|Something else|Not reported</t>
-        </is>
-      </c>
       <c r="H10" t="inlineStr">
         <is>
+          <t>gender_id_condensed</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
           <t>Gender Identity (condensed)</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>gender_id_condensed</t>
-        </is>
-      </c>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr">
         <is>
@@ -1116,562 +1116,562 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>d3_white</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>boolean</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>[White] What is your race? SELECT ALL THAT APPLY</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>d3_white</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>boolean</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>[White] What is your race? SELECT ALL THAT APPLY</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
+          <t>race_white</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
           <t>Race: White</t>
         </is>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>1</v>
       </c>
-      <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>race_white</t>
-        </is>
-      </c>
+      <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>d3_black</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>boolean</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>[Black or African American] What is your race? SELECT ALL THAT APPLY</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>d3_black</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>boolean</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>[Black or African American] What is your race? SELECT ALL THAT APPLY</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
+          <t>race_black</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
           <t>Race: Black or African American</t>
         </is>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>1</v>
       </c>
-      <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>race_black</t>
-        </is>
-      </c>
+      <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>d3_american_indian</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>boolean</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>[American Indian or Alaska Native] What is your race? SELECT ALL THAT APPLY</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>d3_american_indian</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>boolean</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>[American Indian or Alaska Native] What is your race? SELECT ALL THAT APPLY</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
+          <t>race_AIAN</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
           <t>Race: American Indian or Alaska Native</t>
         </is>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>1</v>
       </c>
-      <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>race_AIAN</t>
-        </is>
-      </c>
+      <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>d3_hawaiian</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>boolean</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>[Native Hawaiian or Other Pacific Islander] What is your race? SELECT ALL THAT APPLY</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>d3_hawaiian</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>boolean</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>[Native Hawaiian or Other Pacific Islander] What is your race? SELECT ALL THAT APPLY</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
+          <t>race_hawaiian_OPI</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
           <t>Race: Native Hawaiian or Other Pacific Islander</t>
         </is>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>1</v>
       </c>
-      <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>race_hawaiian_OPI</t>
-        </is>
-      </c>
+      <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>d3_asian</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>boolean</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>[Asian] What is your race? SELECT ALL THAT APPLY</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>d3_asian</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>boolean</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>[Asian] What is your race? SELECT ALL THAT APPLY</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
+          <t>race_asian</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
           <t>Race: Asian</t>
         </is>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>1</v>
       </c>
-      <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>race_asian</t>
-        </is>
-      </c>
+      <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>d3_other</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>boolean</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>[Other] What is your race? SELECT ALL THAT APPLY</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>d3_other</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>boolean</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>[Other] What is your race? SELECT ALL THAT APPLY</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
+          <t>race_other</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
           <t>Race: Other</t>
         </is>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>1</v>
       </c>
-      <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>race_other</t>
-        </is>
-      </c>
+      <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Demographics</t>
+          <t>d3_specify_tribe</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>d3_specify_tribe</t>
+          <t>string</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
           <t>[American indian principal tribe or community specified] What is your race? SELECT ALL THAT APPLY</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Demographics</t>
+        </is>
+      </c>
       <c r="H17" t="inlineStr">
         <is>
+          <t>race_AI_tribe</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
           <t>Race: American indian principal tribe or community specified</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="n">
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="n">
         <v>80</v>
       </c>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>race_AI_tribe</t>
-        </is>
-      </c>
+      <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Demographics</t>
+          <t>d3_specify_other</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>d3_specify_other</t>
+          <t>string</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
           <t>[Other specified] What is your race? SELECT ALL THAT APPLY</t>
         </is>
       </c>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Demographics</t>
+        </is>
+      </c>
       <c r="H18" t="inlineStr">
         <is>
+          <t>race_other_specified</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
           <t>Race: Other specified</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="n">
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="n">
         <v>80</v>
       </c>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>race_other_specified</t>
-        </is>
-      </c>
+      <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>d2</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>boolean</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Are you of Hispanic, Latino, or Spanish origin?</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>d2</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>boolean</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Are you of Hispanic, Latino, or Spanish origin?</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
+          <t>hispanic_latino</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
           <t>Hispanic, Latino, or Spanish Origin</t>
         </is>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>1</v>
       </c>
-      <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>hispanic_latino</t>
-        </is>
-      </c>
+      <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>d4c</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Sexual orientation:  Do you think of yourself as…</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Straight or heterosexual|Lesbian or gay|Bisexual|Queer,pansexual, and/or questioning|Something else</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>d4c</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Sexual orientation:  Do you think of yourself as…</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Straight or heterosexual|Lesbian or gay|Bisexual|Queer,pansexual, and/or questioning|Something else</t>
-        </is>
-      </c>
       <c r="H20" t="inlineStr">
         <is>
+          <t>sex_orient_category</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
           <t>Sexual orientation</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>sex_orient_category</t>
-        </is>
-      </c>
+      <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Demographics</t>
+          <t>d4c_specify_other</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>d4c_specify_other</t>
+          <t>string</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
           <t>Sexual orientation:  Do you think of yourself as…</t>
         </is>
       </c>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Demographics</t>
+        </is>
+      </c>
       <c r="H21" t="inlineStr">
         <is>
+          <t>sex_orient_other</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
           <t>Sexual orientation:  Other specified</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>sex_orient_other</t>
-        </is>
-      </c>
+      <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>d4d</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Have you ever been pregnant?</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Never been pregnant|Currently pregnant|Previously pregnant, had a child|Previously pregnant, did not have a child|Not applicable|Don't know</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>d4d</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Have you ever been pregnant?</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Never been pregnant|Currently pregnant|Previously pregnant, had a child|Previously pregnant, did not have a child|Not applicable|Don't know</t>
-        </is>
-      </c>
       <c r="H22" t="inlineStr">
         <is>
+          <t>ever_pregnant</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
           <t>Ever pregnant</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>ever_pregnant</t>
-        </is>
-      </c>
+      <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr">
         <is>
@@ -1682,668 +1682,668 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>d5</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>What is your marital status?</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Married|Widowed|Divorced|Separated|Never married</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>d5</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>What is your marital status?</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Married|Widowed|Divorced|Separated|Never married</t>
-        </is>
-      </c>
       <c r="H23" t="inlineStr">
         <is>
+          <t>marital_status</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
           <t>Marital status</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>marital_status</t>
-        </is>
-      </c>
+      <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>d5a</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Are you currently living as married with a romantic partner?</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Yes, I am living as married with partner|No, I am not living as married with partner</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>d5a</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Are you currently living as married with a romantic partner?</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Yes, I am living as married with partner|No, I am not living as married with partner</t>
-        </is>
-      </c>
       <c r="H24" t="inlineStr">
         <is>
+          <t>living_as_married</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
           <t>Married with partner</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>living_as_married</t>
-        </is>
-      </c>
+      <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>d6</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>What is the highest grade or level of school you have completed or the highest degree you have received?</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Did not complete high school|GED or equivalent|Regular high school diploma|Some college credit but less than 1 year of college credit|1 or more years of college credit but no degree|Associate's degree (e.g., AA or AS)|Bachelor's degree (e.g.,  BA or BS)|Graduate degree (e.g., MSW, MA, MS, JD, MD, DSW, EdD, PhD)|Other (specify)</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
           <t>Demographics</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>d6</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>What is the highest grade or level of school you have completed or the highest degree you have received?</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>Did not complete high school|GED or equivalent|Regular high school diploma|Some college credit but less than 1 year of college credit|1 or more years of college credit but no degree|Associate's degree (e.g., AA or AS)|Bachelor's degree (e.g.,  BA or BS)|Graduate degree (e.g., MSW, MA, MS, JD, MD, DSW, EdD, PhD)|Other (specify)</t>
-        </is>
-      </c>
       <c r="H25" t="inlineStr">
         <is>
+          <t>educ_category</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
           <t>Education</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>educ_category</t>
-        </is>
-      </c>
+      <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Demographics</t>
+          <t>d6_grade</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>d6_grade</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>integer</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
           <t>What is the highest grade completed?</t>
         </is>
       </c>
+      <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Demographics</t>
+        </is>
+      </c>
       <c r="H26" t="inlineStr">
         <is>
+          <t>educ_highest_grade</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
           <t>Education:  Highest grade level (if less than GED or h.s. diploma)</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>educ_highest_grade</t>
-        </is>
-      </c>
+      <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Demographics</t>
+          <t>d6_specify_other</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>d6_specify_other</t>
+          <t>string</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
           <t>What is the highest grade or level of school you have completed or the highest degree you have received?</t>
         </is>
       </c>
+      <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Demographics</t>
+        </is>
+      </c>
       <c r="H27" t="inlineStr">
         <is>
+          <t>educ_other_specified</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
           <t>Education: Other specified</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>educ_other_specified</t>
-        </is>
-      </c>
+      <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>u14f</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>boolean</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Interview conducted with participant during incarceration?</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
+        <is>
           <t>MOUD</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>u14f</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>boolean</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Interview conducted with participant during incarceration?</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
+          <t>intv_while_incarc</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
           <t>Interviewed during incarceration</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>intv_while_incarc</t>
-        </is>
-      </c>
+      <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>MOUD</t>
+          <t>u14g</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>u14g</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>integer</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
           <t>During the past xx/30 days, how many days have you been incarcerated?</t>
         </is>
       </c>
+      <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>MOUD</t>
+        </is>
+      </c>
       <c r="H29" t="inlineStr">
         <is>
+          <t>days_incarcerated_interval</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
           <t>Days incarcerated (in past 30/xx days)</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>days_incarcerated_interval</t>
-        </is>
-      </c>
+      <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>u15</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>boolean</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Have you ever been prescribed and taken medication to treat opioid use disorder?  (Illicit use should be excluded.)</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr">
+        <is>
           <t>MOUD</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>u15</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>boolean</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Have you ever been prescribed and taken medication to treat opioid use disorder?  (Illicit use should be excluded.)</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
+          <t>ever_rx_moud</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
           <t>Medication ever prescribed for opioid use disorder?</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>ever_rx_moud</t>
-        </is>
-      </c>
+      <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>MOUD</t>
+          <t>u15a1</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>u15a1</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>integer</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
           <t>Lifetime months (buprenorphine-naloxone or buprenorphine daily sublingual [e.g., Suboxone film or tablet, generic films or tablets, or Subutex tablets])</t>
         </is>
       </c>
+      <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>MOUD</t>
+        </is>
+      </c>
       <c r="H31" t="inlineStr">
         <is>
+          <t>months_daily_bup</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
           <t>Buprenorphine-naloxone or buprenorphine daily sublingual: Lifetime months</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>months_daily_bup</t>
-        </is>
-      </c>
+      <c r="L31" t="inlineStr"/>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>MOUD</t>
+          <t>u15b1</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>u15b1</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>integer</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
           <t>Lifetime months (buprenorphine injection [Sublocade])</t>
         </is>
       </c>
+      <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>MOUD</t>
+        </is>
+      </c>
       <c r="H32" t="inlineStr">
         <is>
+          <t>months_sublocade</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
           <t>Buprenorphine injection (Sublocade):  Lifetime months</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>months_sublocade</t>
-        </is>
-      </c>
+      <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>MOUD</t>
+          <t>u15c1</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>u15c1</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>integer</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
           <t>Lifetime months (buprenorphine weekly injection [Brixadi])</t>
         </is>
       </c>
+      <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>MOUD</t>
+        </is>
+      </c>
       <c r="H33" t="inlineStr">
         <is>
+          <t>months_weekly_brixadi</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
           <t>Buprenorphine  weekly injection (Brixadi):  Lifetime months</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>months_weekly_brixadi</t>
-        </is>
-      </c>
+      <c r="L33" t="inlineStr"/>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>MOUD</t>
+          <t>u15d1</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>u15d1</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>integer</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
           <t>Lifetime months (buprenorphine monthly injection [Brixadi])</t>
         </is>
       </c>
+      <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>MOUD</t>
+        </is>
+      </c>
       <c r="H34" t="inlineStr">
         <is>
+          <t>months_monthly_brixadi</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
           <t>Buprenorphine  monthly injection (Brixadi):  Lifetime months</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr"/>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>months_monthly_brixadi</t>
-        </is>
-      </c>
+      <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>MOUD</t>
+          <t>u15e1</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>u15e1</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>integer</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
           <t>Lifetime months (buprenorphine 6-month implant [Probuphine])</t>
         </is>
       </c>
+      <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>MOUD</t>
+        </is>
+      </c>
       <c r="H35" t="inlineStr">
         <is>
+          <t>months_probuphine_implant</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
           <t>Buprenorphine 6-month implant (Probuphine):  Lifetime months</t>
         </is>
       </c>
-      <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr"/>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>months_probuphine_implant</t>
-        </is>
-      </c>
+      <c r="L35" t="inlineStr"/>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>MOUD</t>
+          <t>u15f1</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>u15f1</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>integer</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
           <t>Lifetime months (Naltrexone daily (oral))</t>
         </is>
       </c>
+      <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>MOUD</t>
+        </is>
+      </c>
       <c r="H36" t="inlineStr">
         <is>
+          <t>months_daily_ntx</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
           <t>Naltrexone daily (oral):  Lifetime months</t>
         </is>
       </c>
-      <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>months_daily_ntx</t>
-        </is>
-      </c>
+      <c r="L36" t="inlineStr"/>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>MOUD</t>
+          <t>u15g1</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>u15g1</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>integer</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
           <t>Lifetime months (Naltrexone monthly injection [Vivitrol])</t>
         </is>
       </c>
+      <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>MOUD</t>
+        </is>
+      </c>
       <c r="H37" t="inlineStr">
         <is>
+          <t>months_monthly_vivitrol</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
           <t>Naltrexone monthly injection (Vivitrol):  Lifetime months</t>
         </is>
       </c>
-      <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>months_monthly_vivitrol</t>
-        </is>
-      </c>
+      <c r="L37" t="inlineStr"/>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>MOUD</t>
+          <t>u15h1</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>u15h1</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>integer</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
           <t>Lifetime months (methadone daily)</t>
         </is>
       </c>
+      <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>MOUD</t>
+        </is>
+      </c>
       <c r="H38" t="inlineStr">
         <is>
+          <t>months_methadone</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
           <t>Methadone daily:  Lifetime months</t>
         </is>
       </c>
-      <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr"/>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>months_methadone</t>
-        </is>
-      </c>
+      <c r="L38" t="inlineStr"/>
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr"/>
     </row>

</xml_diff>